<commit_message>
Add plot functions. Include eredivisie IDs
</commit_message>
<xml_diff>
--- a/opta/data/merged/merged_tournamentschedule.xlsx
+++ b/opta/data/merged/merged_tournamentschedule.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T204"/>
+  <dimension ref="A1:U204"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -530,6 +530,11 @@
         </is>
       </c>
       <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>venue</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>goal_events</t>
         </is>
@@ -596,6 +601,7 @@
       <c r="R2" t="inlineStr"/>
       <c r="S2" t="inlineStr"/>
       <c r="T2" t="inlineStr"/>
+      <c r="U2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -655,6 +661,7 @@
       <c r="R3" t="inlineStr"/>
       <c r="S3" t="inlineStr"/>
       <c r="T3" t="inlineStr"/>
+      <c r="U3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -722,6 +729,7 @@
       <c r="R4" t="inlineStr"/>
       <c r="S4" t="inlineStr"/>
       <c r="T4" t="inlineStr"/>
+      <c r="U4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -779,6 +787,7 @@
       <c r="R5" t="inlineStr"/>
       <c r="S5" t="inlineStr"/>
       <c r="T5" t="inlineStr"/>
+      <c r="U5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -844,6 +853,7 @@
       <c r="R6" t="inlineStr"/>
       <c r="S6" t="inlineStr"/>
       <c r="T6" t="inlineStr"/>
+      <c r="U6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -906,6 +916,7 @@
       <c r="R7" t="inlineStr"/>
       <c r="S7" t="inlineStr"/>
       <c r="T7" t="inlineStr"/>
+      <c r="U7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -966,6 +977,7 @@
       <c r="R8" t="inlineStr"/>
       <c r="S8" t="inlineStr"/>
       <c r="T8" t="inlineStr"/>
+      <c r="U8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -1026,6 +1038,7 @@
       <c r="R9" t="inlineStr"/>
       <c r="S9" t="inlineStr"/>
       <c r="T9" t="inlineStr"/>
+      <c r="U9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -1084,6 +1097,7 @@
       <c r="R10" t="inlineStr"/>
       <c r="S10" t="inlineStr"/>
       <c r="T10" t="inlineStr"/>
+      <c r="U10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -1146,6 +1160,7 @@
       <c r="R11" t="inlineStr"/>
       <c r="S11" t="inlineStr"/>
       <c r="T11" t="inlineStr"/>
+      <c r="U11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -1205,6 +1220,7 @@
       <c r="R12" t="inlineStr"/>
       <c r="S12" t="inlineStr"/>
       <c r="T12" t="inlineStr"/>
+      <c r="U12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -1264,6 +1280,7 @@
       <c r="R13" t="inlineStr"/>
       <c r="S13" t="inlineStr"/>
       <c r="T13" t="inlineStr"/>
+      <c r="U13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -1331,6 +1348,7 @@
       <c r="R14" t="inlineStr"/>
       <c r="S14" t="inlineStr"/>
       <c r="T14" t="inlineStr"/>
+      <c r="U14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -1387,6 +1405,7 @@
       <c r="R15" t="inlineStr"/>
       <c r="S15" t="inlineStr"/>
       <c r="T15" t="inlineStr"/>
+      <c r="U15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -1448,6 +1467,7 @@
       <c r="R16" t="inlineStr"/>
       <c r="S16" t="inlineStr"/>
       <c r="T16" t="inlineStr"/>
+      <c r="U16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -1509,6 +1529,7 @@
       <c r="R17" t="inlineStr"/>
       <c r="S17" t="inlineStr"/>
       <c r="T17" t="inlineStr"/>
+      <c r="U17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -1572,6 +1593,7 @@
       <c r="R18" t="inlineStr"/>
       <c r="S18" t="inlineStr"/>
       <c r="T18" t="inlineStr"/>
+      <c r="U18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="n">
@@ -1633,6 +1655,7 @@
       <c r="R19" t="inlineStr"/>
       <c r="S19" t="inlineStr"/>
       <c r="T19" t="inlineStr"/>
+      <c r="U19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="n">
@@ -1696,6 +1719,7 @@
       <c r="R20" t="inlineStr"/>
       <c r="S20" t="inlineStr"/>
       <c r="T20" t="inlineStr"/>
+      <c r="U20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="n">
@@ -1758,6 +1782,7 @@
       <c r="R21" t="inlineStr"/>
       <c r="S21" t="inlineStr"/>
       <c r="T21" t="inlineStr"/>
+      <c r="U21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="n">
@@ -1815,6 +1840,7 @@
       <c r="R22" t="inlineStr"/>
       <c r="S22" t="inlineStr"/>
       <c r="T22" t="inlineStr"/>
+      <c r="U22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="n">
@@ -1877,6 +1903,7 @@
       <c r="R23" t="inlineStr"/>
       <c r="S23" t="inlineStr"/>
       <c r="T23" t="inlineStr"/>
+      <c r="U23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="n">
@@ -1939,6 +1966,7 @@
       <c r="R24" t="inlineStr"/>
       <c r="S24" t="inlineStr"/>
       <c r="T24" t="inlineStr"/>
+      <c r="U24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="n">
@@ -2001,6 +2029,7 @@
       <c r="R25" t="inlineStr"/>
       <c r="S25" t="inlineStr"/>
       <c r="T25" t="inlineStr"/>
+      <c r="U25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="n">
@@ -2065,6 +2094,7 @@
       <c r="R26" t="inlineStr"/>
       <c r="S26" t="inlineStr"/>
       <c r="T26" t="inlineStr"/>
+      <c r="U26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="n">
@@ -2153,10 +2183,15 @@
       </c>
       <c r="S27" t="inlineStr">
         <is>
-          <t>[['Heerenveen', '4vd2t5schmvvufrfib7f2vjdf', 1, 25, 'S. van Hooijdonk', 'YC'], ['Sparta Rotterdam', '89w5c6pw7vn0dxypi61tt0g4k', 2, 49, 'A. Verschueren', 'YC']]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="T27" t="inlineStr">
+        <is>
+          <t>Abe Lenstra Stadion</t>
+        </is>
+      </c>
+      <c r="U27" t="inlineStr">
         <is>
           <t>[]</t>
         </is>
@@ -2260,7 +2295,12 @@
       </c>
       <c r="T28" t="inlineStr">
         <is>
-          <t>[['Fortuna Sittard', '3ebril33e08ddzob4bhq8awsr', 1, 6, 'P. Gladon'], ['Ajax', 'd0zdg647gvgc95xdtk1vpbkys', 2, 48, 'K. Taylor'], ['Ajax', 'd0zdg647gvgc95xdtk1vpbkys', 2, 51, 'D. Rensch'], ['Ajax', 'd0zdg647gvgc95xdtk1vpbkys', 2, 62, 'B. Brobbey'], ['Fortuna Sittard', '3ebril33e08ddzob4bhq8awsr', 2, 87, 'B. Yılmaz']]</t>
+          <t>Fortuna Sittard Stadion</t>
+        </is>
+      </c>
+      <c r="U28" t="inlineStr">
+        <is>
+          <t>[]</t>
         </is>
       </c>
     </row>
@@ -2356,7 +2396,12 @@
       </c>
       <c r="T29" t="inlineStr">
         <is>
-          <t>[['Excelsior', 'dqk062lu0vm8epvytbm6r4mmf', 1, 10, 'M. Azarkan'], ['Excelsior', 'dqk062lu0vm8epvytbm6r4mmf', 1, 44, 'J. Baas']]</t>
+          <t>Cambuur Stadion</t>
+        </is>
+      </c>
+      <c r="U29" t="inlineStr">
+        <is>
+          <t>[]</t>
         </is>
       </c>
     </row>
@@ -2455,6 +2500,11 @@
       </c>
       <c r="T30" t="inlineStr">
         <is>
+          <t>Philips Stadion</t>
+        </is>
+      </c>
+      <c r="U30" t="inlineStr">
+        <is>
           <t>[['PSV', '24fvcruwqrqvqa3aonf8c3zuy', 1, 18, 'J. Bakayoko'], ['Emmen', '3t0vjqtxc8wpjzv82i3oi2ova', 1, 26, 'M. Kieftenbeld'], ['PSV', '24fvcruwqrqvqa3aonf8c3zuy', 1, 38, 'C. Gakpo'], ['PSV', '24fvcruwqrqvqa3aonf8c3zuy', 2, 54, 'C. Gakpo'], ['Emmen', '3t0vjqtxc8wpjzv82i3oi2ova', 2, 62, 'O. Romeny']]</t>
         </is>
       </c>
@@ -2554,6 +2604,11 @@
       </c>
       <c r="T31" t="inlineStr">
         <is>
+          <t>Mandemakers Stadion</t>
+        </is>
+      </c>
+      <c r="U31" t="inlineStr">
+        <is>
           <t>[['RKC Waalwijk', 'ed5nwjz5za3oyi20nxzgqivmx', 1, 15, 'D. Van den Buijs'], ['RKC Waalwijk', 'ed5nwjz5za3oyi20nxzgqivmx', 1, 45, 'I. Bel Hassani'], ['Utrecht', 'ccpscwdcm65czscrun048ecn5', 2, 52, 'B. Dost'], ['Utrecht', 'ccpscwdcm65czscrun048ecn5', 2, 85, 'B. Dost']]</t>
         </is>
       </c>
@@ -2649,6 +2704,11 @@
         </is>
       </c>
       <c r="T32" t="inlineStr">
+        <is>
+          <t>Euroborg</t>
+        </is>
+      </c>
+      <c r="U32" t="inlineStr">
         <is>
           <t>[['Groningen', 'cos9hxi16eitbcbthof7zrm4m', 1, 2, 'C. Ngonge'], ['Groningen', 'cos9hxi16eitbcbthof7zrm4m', 1, 34, 'J. Strand Larsen'], ['Volendam', '6g9qrm72224jrk6tkxxxi8a9n', 1, 38, 'D. van Mieghem'], ['Volendam', '6g9qrm72224jrk6tkxxxi8a9n', 2, 68, 'B. Benamar']]</t>
         </is>
@@ -2747,6 +2807,11 @@
       </c>
       <c r="T33" t="inlineStr">
         <is>
+          <t>GelreDome</t>
+        </is>
+      </c>
+      <c r="U33" t="inlineStr">
+        <is>
           <t>[['Vitesse', '6hsriqr3ybvyg94w2k19oal50', 1, 19, 'M. Manhoef'], ['Feyenoord', '20vymiy7bo8wkyxai3ew494fz', 1, 31, 'P. Wålemark'], ['Feyenoord', '20vymiy7bo8wkyxai3ew494fz', 1, 41, 'Danilo'], ['Vitesse', '6hsriqr3ybvyg94w2k19oal50', 2, 56, 'N. Frederiksen'], ['Feyenoord', '20vymiy7bo8wkyxai3ew494fz', 2, 61, 'J. Dilrosun'], ['Feyenoord', '20vymiy7bo8wkyxai3ew494fz', 2, 66, 'Danilo'], ['Feyenoord', '20vymiy7bo8wkyxai3ew494fz', 2, 69, 'L. Geertruida']]</t>
         </is>
       </c>
@@ -2840,6 +2905,11 @@
         </is>
       </c>
       <c r="T34" t="inlineStr">
+        <is>
+          <t>Goffertstadion</t>
+        </is>
+      </c>
+      <c r="U34" t="inlineStr">
         <is>
           <t>[['Twente', '4tic29sox7m39fy1ztgv0jsiq', 2, 91, 'S. Steijn']]</t>
         </is>
@@ -2935,6 +3005,11 @@
         </is>
       </c>
       <c r="T35" t="inlineStr">
+        <is>
+          <t>AFAS Stadion</t>
+        </is>
+      </c>
+      <c r="U35" t="inlineStr">
         <is>
           <t>[['AZ', '3kfktv64h7kg7zryax1wktr5r', 2, 70, 'V. Pavlidis'], ['AZ', '3kfktv64h7kg7zryax1wktr5r', 2, 86, 'M. van Brederode']]</t>
         </is>
@@ -3033,6 +3108,11 @@
       </c>
       <c r="T36" t="inlineStr">
         <is>
+          <t>Van Donge &amp; De Roo Stadion</t>
+        </is>
+      </c>
+      <c r="U36" t="inlineStr">
+        <is>
           <t>[['Excelsior', 'dqk062lu0vm8epvytbm6r4mmf', 1, 14, 'R. Kharchouch'], ['Excelsior', 'dqk062lu0vm8epvytbm6r4mmf', 1, 20, 'R. Kharchouch'], ['Vitesse', '6hsriqr3ybvyg94w2k19oal50', 1, 29, 'N. Frederiksen'], ['Excelsior', 'dqk062lu0vm8epvytbm6r4mmf', 2, 76, 'K. Goudmijn']]</t>
         </is>
       </c>
@@ -3130,6 +3210,11 @@
       </c>
       <c r="T37" t="inlineStr">
         <is>
+          <t>De Adelaarshorst</t>
+        </is>
+      </c>
+      <c r="U37" t="inlineStr">
+        <is>
           <t>[['PSV', '24fvcruwqrqvqa3aonf8c3zuy', 1, 3, 'L. de Jong'], ['Go Ahead Eagles', 'b79uipsy57y1jqpy07h4i5ovk', 1, 14, 'I. Lidberg'], ['PSV', '24fvcruwqrqvqa3aonf8c3zuy', 1, 48, 'X. Simons'], ['PSV', '24fvcruwqrqvqa3aonf8c3zuy', 1, 55, 'A. Obispo'], ['PSV', '24fvcruwqrqvqa3aonf8c3zuy', 2, 76, 'X. Simons'], ['Go Ahead Eagles', 'b79uipsy57y1jqpy07h4i5ovk', 2, 80, 'O. Edvardsen'], ['PSV', '24fvcruwqrqvqa3aonf8c3zuy', 2, 89, 'J. Veerman']]</t>
         </is>
       </c>
@@ -3227,6 +3312,11 @@
       </c>
       <c r="T38" t="inlineStr">
         <is>
+          <t>De Oude Meerdijk</t>
+        </is>
+      </c>
+      <c r="U38" t="inlineStr">
+        <is>
           <t>[['Emmen', '3t0vjqtxc8wpjzv82i3oi2ova', 2, 58, 'L. Bernadou'], ['RKC Waalwijk', 'ed5nwjz5za3oyi20nxzgqivmx', 2, 89, 'Julen Lobete']]</t>
         </is>
       </c>
@@ -3318,6 +3408,11 @@
         </is>
       </c>
       <c r="T39" t="inlineStr">
+        <is>
+          <t>Stadion Galgenwaard</t>
+        </is>
+      </c>
+      <c r="U39" t="inlineStr">
         <is>
           <t>[]</t>
         </is>
@@ -3416,6 +3511,11 @@
       </c>
       <c r="T40" t="inlineStr">
         <is>
+          <t>Stadion Feijenoord</t>
+        </is>
+      </c>
+      <c r="U40" t="inlineStr">
+        <is>
           <t>[]</t>
         </is>
       </c>
@@ -3512,6 +3612,11 @@
       </c>
       <c r="T41" t="inlineStr">
         <is>
+          <t>Kras Stadion</t>
+        </is>
+      </c>
+      <c r="U41" t="inlineStr">
+        <is>
           <t>[['Volendam', '6g9qrm72224jrk6tkxxxi8a9n', 1, 11, 'D. van Mieghem'], ['NEC', '8iawijq7s9s6d85mjz8wdslki', 1, 17, 'E. Tavşan'], ['NEC', '8iawijq7s9s6d85mjz8wdslki', 1, 19, 'O. Tannane'], ['NEC', '8iawijq7s9s6d85mjz8wdslki', 2, 76, 'M. Duelund'], ['NEC', '8iawijq7s9s6d85mjz8wdslki', 2, 90, 'J. Bruijn']]</t>
         </is>
       </c>
@@ -3607,6 +3712,11 @@
         </is>
       </c>
       <c r="T42" t="inlineStr">
+        <is>
+          <t>Johan Cruijff Arena</t>
+        </is>
+      </c>
+      <c r="U42" t="inlineStr">
         <is>
           <t>[['Ajax', 'd0zdg647gvgc95xdtk1vpbkys', 1, 4, 'S. Bergwijn'], ['Groningen', 'cos9hxi16eitbcbthof7zrm4m', 1, 10, 'C. Ngonge'], ['Ajax', 'd0zdg647gvgc95xdtk1vpbkys', 1, 28, 'Antony'], ['Ajax', 'd0zdg647gvgc95xdtk1vpbkys', 1, 45, 'S. Bergwijn'], ['Ajax', 'd0zdg647gvgc95xdtk1vpbkys', 2, 57, 'S. Bergwijn'], ['Ajax', 'd0zdg647gvgc95xdtk1vpbkys', 2, 66, 'K. Taylor'], ['Ajax', 'd0zdg647gvgc95xdtk1vpbkys', 2, 88, 'S. Berghuis']]</t>
         </is>
@@ -3705,6 +3815,11 @@
         </is>
       </c>
       <c r="T43" t="inlineStr">
+        <is>
+          <t>De Grolsch Veste</t>
+        </is>
+      </c>
+      <c r="U43" t="inlineStr">
         <is>
           <t>[['Twente', '4tic29sox7m39fy1ztgv0jsiq', 1, 22, 'R. van Wolfswinkel'], ['Twente', '4tic29sox7m39fy1ztgv0jsiq', 1, 44, 'J. Brenet'], ['Twente', '4tic29sox7m39fy1ztgv0jsiq', 2, 53, 'V. Misidjan']]</t>
         </is>
@@ -3805,6 +3920,11 @@
       </c>
       <c r="T44" t="inlineStr">
         <is>
+          <t>Sparta-Stadion Het Kasteel</t>
+        </is>
+      </c>
+      <c r="U44" t="inlineStr">
+        <is>
           <t>[['Sparta Rotterdam', '89w5c6pw7vn0dxypi61tt0g4k', 1, 1, 'V. van Crooij'], ['AZ', '3kfktv64h7kg7zryax1wktr5r', 1, 46, 'V. Pavlidis'], ['AZ', '3kfktv64h7kg7zryax1wktr5r', 2, 57, 'D. de Wit'], ['Sparta Rotterdam', '89w5c6pw7vn0dxypi61tt0g4k', 2, 59, 'V. van Crooij'], ['AZ', '3kfktv64h7kg7zryax1wktr5r', 2, 65, 'M. Kerkez']]</t>
         </is>
       </c>
@@ -3904,6 +4024,11 @@
       </c>
       <c r="T45" t="inlineStr">
         <is>
+          <t>GelreDome</t>
+        </is>
+      </c>
+      <c r="U45" t="inlineStr">
+        <is>
           <t>[['Heerenveen', '4vd2t5schmvvufrfib7f2vjdf', 1, 5, 'S. van Hooijdonk'], ['Heerenveen', '4vd2t5schmvvufrfib7f2vjdf', 1, 48, 'A. Sarr'], ['Heerenveen', '4vd2t5schmvvufrfib7f2vjdf', 2, 72, 'S. van Hooijdonk'], ['Heerenveen', '4vd2t5schmvvufrfib7f2vjdf', 2, 77, 'S. van Hooijdonk']]</t>
         </is>
       </c>
@@ -3997,6 +4122,11 @@
         </is>
       </c>
       <c r="T46" t="inlineStr">
+        <is>
+          <t>Euroborg</t>
+        </is>
+      </c>
+      <c r="U46" t="inlineStr">
         <is>
           <t>[['Go Ahead Eagles', 'b79uipsy57y1jqpy07h4i5ovk', 1, 3, 'J. de Lange']]</t>
         </is>
@@ -4095,6 +4225,11 @@
       </c>
       <c r="T47" t="inlineStr">
         <is>
+          <t>Philips Stadion</t>
+        </is>
+      </c>
+      <c r="U47" t="inlineStr">
+        <is>
           <t>[['PSV', '24fvcruwqrqvqa3aonf8c3zuy', 1, 1, 'X. Simons'], ['PSV', '24fvcruwqrqvqa3aonf8c3zuy', 1, 25, 'C. Gakpo'], ['PSV', '24fvcruwqrqvqa3aonf8c3zuy', 1, 39, 'C. Gakpo'], ['Volendam', '6g9qrm72224jrk6tkxxxi8a9n', 1, 40, 'H. Veerman'], ['Volendam', '6g9qrm72224jrk6tkxxxi8a9n', 2, 47, 'B. Plat'], ['PSV', '24fvcruwqrqvqa3aonf8c3zuy', 2, 51, 'C. Gakpo'], ['PSV', '24fvcruwqrqvqa3aonf8c3zuy', 2, 67, 'X. Simons'], ['PSV', '24fvcruwqrqvqa3aonf8c3zuy', 2, 79, 'J. Bakayoko']]</t>
         </is>
       </c>
@@ -4186,6 +4321,11 @@
         </is>
       </c>
       <c r="T48" t="inlineStr">
+        <is>
+          <t>AFAS Stadion</t>
+        </is>
+      </c>
+      <c r="U48" t="inlineStr">
         <is>
           <t>[['NEC', '8iawijq7s9s6d85mjz8wdslki', 2, 54, 'Iván Márquez'], ['AZ', '3kfktv64h7kg7zryax1wktr5r', 2, 57, 'J. Odgaard']]</t>
         </is>
@@ -4282,6 +4422,11 @@
         </is>
       </c>
       <c r="T49" t="inlineStr">
+        <is>
+          <t>Sparta-Stadion Het Kasteel</t>
+        </is>
+      </c>
+      <c r="U49" t="inlineStr">
         <is>
           <t>[['Ajax', 'd0zdg647gvgc95xdtk1vpbkys', 1, 37, 'S. Bergwijn']]</t>
         </is>
@@ -4382,6 +4527,11 @@
       </c>
       <c r="T50" t="inlineStr">
         <is>
+          <t>Mandemakers Stadion</t>
+        </is>
+      </c>
+      <c r="U50" t="inlineStr">
+        <is>
           <t>[['Feyenoord', '20vymiy7bo8wkyxai3ew494fz', 2, 68, 'Danilo']]</t>
         </is>
       </c>
@@ -4476,6 +4626,11 @@
       </c>
       <c r="T51" t="inlineStr">
         <is>
+          <t>Goffertstadion</t>
+        </is>
+      </c>
+      <c r="U51" t="inlineStr">
+        <is>
           <t>[['Groningen', 'cos9hxi16eitbcbthof7zrm4m', 2, 75, 'L. Duarte'], ['NEC', '8iawijq7s9s6d85mjz8wdslki', 2, 88, 'I. Cissoko']]</t>
         </is>
       </c>
@@ -4569,6 +4724,11 @@
         </is>
       </c>
       <c r="T52" t="inlineStr">
+        <is>
+          <t>De Adelaarshorst</t>
+        </is>
+      </c>
+      <c r="U52" t="inlineStr">
         <is>
           <t>[['Sparta Rotterdam', '89w5c6pw7vn0dxypi61tt0g4k', 1, 18, 'T. Lauritsen']]</t>
         </is>
@@ -4667,6 +4827,11 @@
       </c>
       <c r="T53" t="inlineStr">
         <is>
+          <t>GelreDome</t>
+        </is>
+      </c>
+      <c r="U53" t="inlineStr">
+        <is>
           <t>[['RKC Waalwijk', 'ed5nwjz5za3oyi20nxzgqivmx', 1, 35, 'F. Jozefzoon'], ['RKC Waalwijk', 'ed5nwjz5za3oyi20nxzgqivmx', 2, 50, 'I. Bel Hassani'], ['Vitesse', '6hsriqr3ybvyg94w2k19oal50', 2, 61, 'M. Bero'], ['Vitesse', '6hsriqr3ybvyg94w2k19oal50', 2, 71, 'R. Flamingo']]</t>
         </is>
       </c>
@@ -4760,6 +4925,11 @@
         </is>
       </c>
       <c r="T54" t="inlineStr">
+        <is>
+          <t>Stadion Feijenoord</t>
+        </is>
+      </c>
+      <c r="U54" t="inlineStr">
         <is>
           <t>[['Feyenoord', '20vymiy7bo8wkyxai3ew494fz', 2, 60, 'Q. Timber'], ['Feyenoord', '20vymiy7bo8wkyxai3ew494fz', 2, 85, 'S. Giménez'], ['Feyenoord', '20vymiy7bo8wkyxai3ew494fz', 2, 88, 'J. Rasmussen'], ['Feyenoord', '20vymiy7bo8wkyxai3ew494fz', 2, 92, 'S. Szymański']]</t>
         </is>
@@ -4857,6 +5027,11 @@
         </is>
       </c>
       <c r="T55" t="inlineStr">
+        <is>
+          <t>Abe Lenstra Stadion</t>
+        </is>
+      </c>
+      <c r="U55" t="inlineStr">
         <is>
           <t>[['Heerenveen', '4vd2t5schmvvufrfib7f2vjdf', 1, 22, 'S. van Hooijdonk'], ['Heerenveen', '4vd2t5schmvvufrfib7f2vjdf', 1, 44, 'M. van Ewijk'], ['Fortuna Sittard', '3ebril33e08ddzob4bhq8awsr', 2, 84, 'B. Yılmaz']]</t>
         </is>
@@ -4958,6 +5133,11 @@
       </c>
       <c r="T56" t="inlineStr">
         <is>
+          <t>Stadion Galgenwaard</t>
+        </is>
+      </c>
+      <c r="U56" t="inlineStr">
+        <is>
           <t>[['Ajax', 'd0zdg647gvgc95xdtk1vpbkys', 1, 10, 'S. Berghuis'], ['Ajax', 'd0zdg647gvgc95xdtk1vpbkys', 1, 46, 'B. Brobbey']]</t>
         </is>
       </c>
@@ -5054,6 +5234,11 @@
       </c>
       <c r="T57" t="inlineStr">
         <is>
+          <t>Van Donge &amp; De Roo Stadion</t>
+        </is>
+      </c>
+      <c r="U57" t="inlineStr">
+        <is>
           <t>[['PSV', '24fvcruwqrqvqa3aonf8c3zuy', 1, 2, 'J. Veerman'], ['PSV', '24fvcruwqrqvqa3aonf8c3zuy', 1, 29, 'I. Sangaré'], ['PSV', '24fvcruwqrqvqa3aonf8c3zuy', 1, 45, 'I. Sangaré'], ['PSV', '24fvcruwqrqvqa3aonf8c3zuy', 2, 55, 'X. Simons'], ['PSV', '24fvcruwqrqvqa3aonf8c3zuy', 2, 59, 'C. Gakpo'], ['Excelsior', 'dqk062lu0vm8epvytbm6r4mmf', 2, 74, 'S. Horemans'], ['PSV', '24fvcruwqrqvqa3aonf8c3zuy', 2, 84, 'X. Simons']]</t>
         </is>
       </c>
@@ -5149,6 +5334,11 @@
       </c>
       <c r="T58" t="inlineStr">
         <is>
+          <t>Kras Stadion</t>
+        </is>
+      </c>
+      <c r="U58" t="inlineStr">
+        <is>
           <t>[['Volendam', '6g9qrm72224jrk6tkxxxi8a9n', 2, 83, 'L. Zeefuik']]</t>
         </is>
       </c>
@@ -5243,6 +5433,11 @@
         </is>
       </c>
       <c r="T59" t="inlineStr">
+        <is>
+          <t>Cambuur Stadion</t>
+        </is>
+      </c>
+      <c r="U59" t="inlineStr">
         <is>
           <t>[['AZ', '3kfktv64h7kg7zryax1wktr5r', 2, 90, 'J. Clasie']]</t>
         </is>
@@ -5339,6 +5534,11 @@
         </is>
       </c>
       <c r="T60" t="inlineStr">
+        <is>
+          <t>De Grolsch Veste</t>
+        </is>
+      </c>
+      <c r="U60" t="inlineStr">
         <is>
           <t>[['Twente', '4tic29sox7m39fy1ztgv0jsiq', 1, 1, 'D. Cleonise'], ['Twente', '4tic29sox7m39fy1ztgv0jsiq', 1, 8, 'C. Tzolis'], ['Twente', '4tic29sox7m39fy1ztgv0jsiq', 2, 62, 'V. Černý'], ['Twente', '4tic29sox7m39fy1ztgv0jsiq', 2, 93, 'V. Černý']]</t>
         </is>
@@ -5442,6 +5642,11 @@
       </c>
       <c r="T61" t="inlineStr">
         <is>
+          <t>Fortuna Sittard Stadion</t>
+        </is>
+      </c>
+      <c r="U61" t="inlineStr">
+        <is>
           <t>[['Utrecht', 'ccpscwdcm65czscrun048ecn5', 2, 64, 'B. Dost'], ['Fortuna Sittard', '3ebril33e08ddzob4bhq8awsr', 2, 67, 'Rodrigo Guth'], ['Utrecht', 'ccpscwdcm65czscrun048ecn5', 2, 70, 'T. Douvikas'], ['Utrecht', 'ccpscwdcm65czscrun048ecn5', 2, 77, 'T. Douvikas'], ['Fortuna Sittard', '3ebril33e08ddzob4bhq8awsr', 2, 82, 'B. Yılmaz'], ['Utrecht', 'ccpscwdcm65czscrun048ecn5', 2, 86, 'T. Douvikas'], ['Fortuna Sittard', '3ebril33e08ddzob4bhq8awsr', 2, 97, 'T. Noslin']]</t>
         </is>
       </c>
@@ -5544,6 +5749,11 @@
       </c>
       <c r="T62" t="inlineStr">
         <is>
+          <t>Johan Cruijff Arena</t>
+        </is>
+      </c>
+      <c r="U62" t="inlineStr">
+        <is>
           <t>[['Ajax', 'd0zdg647gvgc95xdtk1vpbkys', 1, 35, 'S. Bergwijn'], ['Ajax', 'd0zdg647gvgc95xdtk1vpbkys', 1, 40, 'S. Bergwijn'], ['Ajax', 'd0zdg647gvgc95xdtk1vpbkys', 2, 53, 'D. Rensch'], ['Ajax', 'd0zdg647gvgc95xdtk1vpbkys', 2, 64, 'M. Kudus']]</t>
         </is>
       </c>
@@ -5643,6 +5853,11 @@
       </c>
       <c r="T63" t="inlineStr">
         <is>
+          <t>De Grolsch Veste</t>
+        </is>
+      </c>
+      <c r="U63" t="inlineStr">
+        <is>
           <t>[['Twente', '4tic29sox7m39fy1ztgv0jsiq', 1, 17, 'V. Černý'], ['Twente', '4tic29sox7m39fy1ztgv0jsiq', 1, 24, 'V. Černý'], ['PSV', '24fvcruwqrqvqa3aonf8c3zuy', 2, 55, 'G. Til']]</t>
         </is>
       </c>
@@ -5740,6 +5955,11 @@
         </is>
       </c>
       <c r="T64" t="inlineStr">
+        <is>
+          <t>Sparta-Stadion Het Kasteel</t>
+        </is>
+      </c>
+      <c r="U64" t="inlineStr">
         <is>
           <t>[['Sparta Rotterdam', '89w5c6pw7vn0dxypi61tt0g4k', 1, 14, 'V. van Crooij'], ['Sparta Rotterdam', '89w5c6pw7vn0dxypi61tt0g4k', 2, 68, 'T. Lauritsen'], ['Sparta Rotterdam', '89w5c6pw7vn0dxypi61tt0g4k', 2, 72, 'T. Lauritsen'], ['Sparta Rotterdam', '89w5c6pw7vn0dxypi61tt0g4k', 2, 85, 'S. Mijnans']]</t>
         </is>
@@ -5841,6 +6061,11 @@
       </c>
       <c r="T65" t="inlineStr">
         <is>
+          <t>De Adelaarshorst</t>
+        </is>
+      </c>
+      <c r="U65" t="inlineStr">
+        <is>
           <t>[['Feyenoord', '20vymiy7bo8wkyxai3ew494fz', 1, 3, 'P. Wålemark'], ['Go Ahead Eagles', 'b79uipsy57y1jqpy07h4i5ovk', 1, 13, 'I. Lidberg'], ['Feyenoord', '20vymiy7bo8wkyxai3ew494fz', 1, 24, 'Danilo'], ['Feyenoord', '20vymiy7bo8wkyxai3ew494fz', 1, 42, 'Danilo'], ['Feyenoord', '20vymiy7bo8wkyxai3ew494fz', 2, 56, 'J. Dilrosun'], ['Feyenoord', '20vymiy7bo8wkyxai3ew494fz', 2, 79, 'S. Szymański'], ['Go Ahead Eagles', 'b79uipsy57y1jqpy07h4i5ovk', 2, 96, 'O. Edvardsen']]</t>
         </is>
       </c>
@@ -5938,6 +6163,11 @@
       </c>
       <c r="T66" t="inlineStr">
         <is>
+          <t>Mandemakers Stadion</t>
+        </is>
+      </c>
+      <c r="U66" t="inlineStr">
+        <is>
           <t>[['Excelsior', 'dqk062lu0vm8epvytbm6r4mmf', 1, 15, 'J. Baas'], ['RKC Waalwijk', 'ed5nwjz5za3oyi20nxzgqivmx', 1, 38, 'S. Adewoye'], ['Excelsior', 'dqk062lu0vm8epvytbm6r4mmf', 1, 43, 'R. El Yaakoubi'], ['RKC Waalwijk', 'ed5nwjz5za3oyi20nxzgqivmx', 2, 50, 'P. Clement'], ['RKC Waalwijk', 'ed5nwjz5za3oyi20nxzgqivmx', 2, 60, 'T. Lutonda'], ['RKC Waalwijk', 'ed5nwjz5za3oyi20nxzgqivmx', 2, 80, 'V. Anita'], ['RKC Waalwijk', 'ed5nwjz5za3oyi20nxzgqivmx', 2, 91, 'M. Kramer']]</t>
         </is>
       </c>
@@ -6034,6 +6264,11 @@
       </c>
       <c r="T67" t="inlineStr">
         <is>
+          <t>De Oude Meerdijk</t>
+        </is>
+      </c>
+      <c r="U67" t="inlineStr">
+        <is>
           <t>[['AZ', '3kfktv64h7kg7zryax1wktr5r', 1, 21, 'J. Odgaard'], ['AZ', '3kfktv64h7kg7zryax1wktr5r', 1, 27, 'D. de Wit'], ['AZ', '3kfktv64h7kg7zryax1wktr5r', 1, 34, 'T. Reijnders']]</t>
         </is>
       </c>
@@ -6129,6 +6364,11 @@
         </is>
       </c>
       <c r="T68" t="inlineStr">
+        <is>
+          <t>Abe Lenstra Stadion</t>
+        </is>
+      </c>
+      <c r="U68" t="inlineStr">
         <is>
           <t>[]</t>
         </is>
@@ -6229,6 +6469,11 @@
       </c>
       <c r="T69" t="inlineStr">
         <is>
+          <t>Euroborg</t>
+        </is>
+      </c>
+      <c r="U69" t="inlineStr">
+        <is>
           <t>[['Vitesse', '6hsriqr3ybvyg94w2k19oal50', 2, 77, 'M. Bero']]</t>
         </is>
       </c>
@@ -6326,6 +6571,11 @@
       </c>
       <c r="T70" t="inlineStr">
         <is>
+          <t>Kras Stadion</t>
+        </is>
+      </c>
+      <c r="U70" t="inlineStr">
+        <is>
           <t>[['Go Ahead Eagles', 'b79uipsy57y1jqpy07h4i5ovk', 1, 23, 'B. Adekanye'], ['Volendam', '6g9qrm72224jrk6tkxxxi8a9n', 1, 31, 'C. Eiting'], ['Go Ahead Eagles', 'b79uipsy57y1jqpy07h4i5ovk', 2, 77, 'B. Kuipers'], ['Go Ahead Eagles', 'b79uipsy57y1jqpy07h4i5ovk', 2, 82, 'B. Kuipers'], ['Volendam', '6g9qrm72224jrk6tkxxxi8a9n', 2, 97, 'R. Mühren']]</t>
         </is>
       </c>
@@ -6421,6 +6671,11 @@
         </is>
       </c>
       <c r="T71" t="inlineStr">
+        <is>
+          <t>Goffertstadion</t>
+        </is>
+      </c>
+      <c r="U71" t="inlineStr">
         <is>
           <t>[['Fortuna Sittard', '3ebril33e08ddzob4bhq8awsr', 2, 71, 'O. Özyakup'], ['NEC', '8iawijq7s9s6d85mjz8wdslki', 2, 95, 'Pedro Marques']]</t>
         </is>
@@ -6522,6 +6777,11 @@
       </c>
       <c r="T72" t="inlineStr">
         <is>
+          <t>Johan Cruijff Arena</t>
+        </is>
+      </c>
+      <c r="U72" t="inlineStr">
+        <is>
           <t>[['Ajax', 'd0zdg647gvgc95xdtk1vpbkys', 1, 4, 'D. Klaassen'], ['Ajax', 'd0zdg647gvgc95xdtk1vpbkys', 1, 16, 'K. Taylor'], ['Ajax', 'd0zdg647gvgc95xdtk1vpbkys', 2, 48, 'M. Kudus'], ['Ajax', 'd0zdg647gvgc95xdtk1vpbkys', 2, 59, 'M. Kudus'], ['Ajax', 'd0zdg647gvgc95xdtk1vpbkys', 2, 70, 'B. Brobbey']]</t>
         </is>
       </c>
@@ -6616,6 +6876,11 @@
         </is>
       </c>
       <c r="T73" t="inlineStr">
+        <is>
+          <t>Van Donge &amp; De Roo Stadion</t>
+        </is>
+      </c>
+      <c r="U73" t="inlineStr">
         <is>
           <t>[['Emmen', '3t0vjqtxc8wpjzv82i3oi2ova', 1, 45, 'O. Romeny'], ['Excelsior', 'dqk062lu0vm8epvytbm6r4mmf', 2, 61, 'N. Tjoe-A-On'], ['Excelsior', 'dqk062lu0vm8epvytbm6r4mmf', 2, 95, 'S. Seymor']]</t>
         </is>
@@ -6714,6 +6979,11 @@
       </c>
       <c r="T74" t="inlineStr">
         <is>
+          <t>Philips Stadion</t>
+        </is>
+      </c>
+      <c r="U74" t="inlineStr">
+        <is>
           <t>[['PSV', '24fvcruwqrqvqa3aonf8c3zuy', 2, 96, 'C. Gakpo']]</t>
         </is>
       </c>
@@ -6811,6 +7081,11 @@
       </c>
       <c r="T75" t="inlineStr">
         <is>
+          <t>Stadion Galgenwaard</t>
+        </is>
+      </c>
+      <c r="U75" t="inlineStr">
+        <is>
           <t>[['Utrecht', 'ccpscwdcm65czscrun048ecn5', 2, 84, 'B. Dost']]</t>
         </is>
       </c>
@@ -6906,6 +7181,11 @@
       </c>
       <c r="T76" t="inlineStr">
         <is>
+          <t>Cambuur Stadion</t>
+        </is>
+      </c>
+      <c r="U76" t="inlineStr">
+        <is>
           <t>[['Groningen', 'cos9hxi16eitbcbthof7zrm4m', 2, 71, 'T. Suslov']]</t>
         </is>
       </c>
@@ -7000,6 +7280,11 @@
         </is>
       </c>
       <c r="T77" t="inlineStr">
+        <is>
+          <t>Stadion Feijenoord</t>
+        </is>
+      </c>
+      <c r="U77" t="inlineStr">
         <is>
           <t>[['Feyenoord', '20vymiy7bo8wkyxai3ew494fz', 1, 5, 'O. Kökçü'], ['Feyenoord', '20vymiy7bo8wkyxai3ew494fz', 1, 35, 'J. Dilrosun'], ['Feyenoord', '20vymiy7bo8wkyxai3ew494fz', 2, 73, 'S. Giménez']]</t>
         </is>
@@ -7098,6 +7383,11 @@
       </c>
       <c r="T78" t="inlineStr">
         <is>
+          <t>Stadion Galgenwaard</t>
+        </is>
+      </c>
+      <c r="U78" t="inlineStr">
+        <is>
           <t>[]</t>
         </is>
       </c>
@@ -7193,6 +7483,11 @@
         </is>
       </c>
       <c r="T79" t="inlineStr">
+        <is>
+          <t>Sparta-Stadion Het Kasteel</t>
+        </is>
+      </c>
+      <c r="U79" t="inlineStr">
         <is>
           <t>[['Groningen', 'cos9hxi16eitbcbthof7zrm4m', 2, 61, 'R. Pepi'], ['Sparta Rotterdam', '89w5c6pw7vn0dxypi61tt0g4k', 2, 73, 'S. Mijnans'], ['Sparta Rotterdam', '89w5c6pw7vn0dxypi61tt0g4k', 2, 90, 'V. van Crooij']]</t>
         </is>
@@ -7291,6 +7586,11 @@
       </c>
       <c r="T80" t="inlineStr">
         <is>
+          <t>GelreDome</t>
+        </is>
+      </c>
+      <c r="U80" t="inlineStr">
+        <is>
           <t>[['Volendam', '6g9qrm72224jrk6tkxxxi8a9n', 1, 21, 'R. Mühren'], ['Vitesse', '6hsriqr3ybvyg94w2k19oal50', 2, 48, 'B. Białek']]</t>
         </is>
       </c>
@@ -7388,6 +7688,11 @@
       </c>
       <c r="T81" t="inlineStr">
         <is>
+          <t>Mandemakers Stadion</t>
+        </is>
+      </c>
+      <c r="U81" t="inlineStr">
+        <is>
           <t>[['Cambuur', 'ears40cp6opsgvhsy0dgyszpd', 1, 17, 'J. Jacobs'], ['RKC Waalwijk', 'ed5nwjz5za3oyi20nxzgqivmx', 1, 32, 'M. Kramer'], ['Cambuur', 'ears40cp6opsgvhsy0dgyszpd', 2, 77, 'M. Tol'], ['RKC Waalwijk', 'ed5nwjz5za3oyi20nxzgqivmx', 2, 82, 'Z. Bakkali'], ['RKC Waalwijk', 'ed5nwjz5za3oyi20nxzgqivmx', 2, 86, 'I. Bel Hassani'], ['RKC Waalwijk', 'ed5nwjz5za3oyi20nxzgqivmx', 2, 89, 'M. Kramer']]</t>
         </is>
       </c>
@@ -7481,6 +7786,11 @@
         </is>
       </c>
       <c r="T82" t="inlineStr">
+        <is>
+          <t>Fortuna Sittard Stadion</t>
+        </is>
+      </c>
+      <c r="U82" t="inlineStr">
         <is>
           <t>[['Fortuna Sittard', '3ebril33e08ddzob4bhq8awsr', 2, 87, 'R. Vita']]</t>
         </is>
@@ -7577,6 +7887,11 @@
         </is>
       </c>
       <c r="T83" t="inlineStr">
+        <is>
+          <t>De Adelaarshorst</t>
+        </is>
+      </c>
+      <c r="U83" t="inlineStr">
         <is>
           <t>[['Go Ahead Eagles', 'b79uipsy57y1jqpy07h4i5ovk', 1, 31, 'O. Edvardsen'], ['Go Ahead Eagles', 'b79uipsy57y1jqpy07h4i5ovk', 2, 57, 'O. Edvardsen']]</t>
         </is>
@@ -7678,6 +7993,11 @@
       </c>
       <c r="T84" t="inlineStr">
         <is>
+          <t>Abe Lenstra Stadion</t>
+        </is>
+      </c>
+      <c r="U84" t="inlineStr">
+        <is>
           <t>[['Twente', '4tic29sox7m39fy1ztgv0jsiq', 1, 2, 'V. Misidjan'], ['Heerenveen', '4vd2t5schmvvufrfib7f2vjdf', 1, 28, 'M. van Ewijk'], ['Heerenveen', '4vd2t5schmvvufrfib7f2vjdf', 1, 36, 'P. Bochniewicz']]</t>
         </is>
       </c>
@@ -7774,6 +8094,11 @@
         </is>
       </c>
       <c r="T85" t="inlineStr">
+        <is>
+          <t>Philips Stadion</t>
+        </is>
+      </c>
+      <c r="U85" t="inlineStr">
         <is>
           <t>[['Feyenoord', '20vymiy7bo8wkyxai3ew494fz', 1, 3, 'O. Idrissi'], ['PSV', '24fvcruwqrqvqa3aonf8c3zuy', 1, 16, 'J. Branthwaite'], ['PSV', '24fvcruwqrqvqa3aonf8c3zuy', 1, 25, 'C. Gakpo'], ['Feyenoord', '20vymiy7bo8wkyxai3ew494fz', 1, 42, 'Danilo'], ['PSV', '24fvcruwqrqvqa3aonf8c3zuy', 2, 47, 'G. Til'], ['Feyenoord', '20vymiy7bo8wkyxai3ew494fz', 2, 73, 'O. Kökçü'], ['PSV', '24fvcruwqrqvqa3aonf8c3zuy', 2, 83, 'A. Obispo']]</t>
         </is>
@@ -7874,6 +8199,11 @@
         </is>
       </c>
       <c r="T86" t="inlineStr">
+        <is>
+          <t>AFAS Stadion</t>
+        </is>
+      </c>
+      <c r="U86" t="inlineStr">
         <is>
           <t>[['Ajax', 'd0zdg647gvgc95xdtk1vpbkys', 1, 12, 'M. Kudus'], ['AZ', '3kfktv64h7kg7zryax1wktr5r', 1, 40, 'M. de Wit'], ['AZ', '3kfktv64h7kg7zryax1wktr5r', 1, 51, 'J. Odgaard']]</t>
         </is>
@@ -7980,6 +8310,11 @@
       </c>
       <c r="T87" t="inlineStr">
         <is>
+          <t>Johan Cruijff Arena</t>
+        </is>
+      </c>
+      <c r="U87" t="inlineStr">
+        <is>
           <t>[['Ajax', 'd0zdg647gvgc95xdtk1vpbkys', 1, 6, 'D. Tadić'], ['Vitesse', '6hsriqr3ybvyg94w2k19oal50', 1, 25, 'M. Manhoef'], ['Vitesse', '6hsriqr3ybvyg94w2k19oal50', 2, 74, 'M. Manhoef'], ['Ajax', 'd0zdg647gvgc95xdtk1vpbkys', 2, 79, 'L. Lucca']]</t>
         </is>
       </c>
@@ -8073,6 +8408,11 @@
         </is>
       </c>
       <c r="T88" t="inlineStr">
+        <is>
+          <t>Stadion Feijenoord</t>
+        </is>
+      </c>
+      <c r="U88" t="inlineStr">
         <is>
           <t>[['Feyenoord', '20vymiy7bo8wkyxai3ew494fz', 1, 4, 'Q. Hartman']]</t>
         </is>
@@ -8170,6 +8510,11 @@
         </is>
       </c>
       <c r="T89" t="inlineStr">
+        <is>
+          <t>Cambuur Stadion</t>
+        </is>
+      </c>
+      <c r="U89" t="inlineStr">
         <is>
           <t>[['NEC', '8iawijq7s9s6d85mjz8wdslki', 1, 44, 'L. Schöne']]</t>
         </is>
@@ -8271,6 +8616,11 @@
       </c>
       <c r="T90" t="inlineStr">
         <is>
+          <t>GelreDome</t>
+        </is>
+      </c>
+      <c r="U90" t="inlineStr">
+        <is>
           <t>[['Sparta Rotterdam', '89w5c6pw7vn0dxypi61tt0g4k', 2, 69, 'T. Lauritsen'], ['Sparta Rotterdam', '89w5c6pw7vn0dxypi61tt0g4k', 2, 72, 'S. Mijnans'], ['Sparta Rotterdam', '89w5c6pw7vn0dxypi61tt0g4k', 2, 88, 'T. Lauritsen'], ['Sparta Rotterdam', '89w5c6pw7vn0dxypi61tt0g4k', 2, 91, 'A. Verschueren']]</t>
         </is>
       </c>
@@ -8367,6 +8717,11 @@
       </c>
       <c r="T91" t="inlineStr">
         <is>
+          <t>Mandemakers Stadion</t>
+        </is>
+      </c>
+      <c r="U91" t="inlineStr">
+        <is>
           <t>[['AZ', '3kfktv64h7kg7zryax1wktr5r', 1, 9, 'J. Karlsson'], ['RKC Waalwijk', 'ed5nwjz5za3oyi20nxzgqivmx', 1, 32, 'I. Bel Hassani'], ['RKC Waalwijk', 'ed5nwjz5za3oyi20nxzgqivmx', 2, 87, 'Z. Bakkali'], ['RKC Waalwijk', 'ed5nwjz5za3oyi20nxzgqivmx', 2, 92, 'Z. Bakkali']]</t>
         </is>
       </c>
@@ -8460,6 +8815,11 @@
         </is>
       </c>
       <c r="T92" t="inlineStr">
+        <is>
+          <t>Fortuna Sittard Stadion</t>
+        </is>
+      </c>
+      <c r="U92" t="inlineStr">
         <is>
           <t>[['Emmen', '3t0vjqtxc8wpjzv82i3oi2ova', 2, 58, 'R. Živković']]</t>
         </is>
@@ -8567,6 +8927,11 @@
       </c>
       <c r="T93" t="inlineStr">
         <is>
+          <t>Johan Cruijff Arena</t>
+        </is>
+      </c>
+      <c r="U93" t="inlineStr">
+        <is>
           <t>[['PSV', '24fvcruwqrqvqa3aonf8c3zuy', 1, 23, 'L. de Jong'], ['PSV', '24fvcruwqrqvqa3aonf8c3zuy', 2, 50, 'É. Gutiérrez'], ['Ajax', 'd0zdg647gvgc95xdtk1vpbkys', 2, 83, 'L. Lucca']]</t>
         </is>
       </c>
@@ -8660,6 +9025,11 @@
         </is>
       </c>
       <c r="T94" t="inlineStr">
+        <is>
+          <t>Van Donge &amp; De Roo Stadion</t>
+        </is>
+      </c>
+      <c r="U94" t="inlineStr">
         <is>
           <t>[['Heerenveen', '4vd2t5schmvvufrfib7f2vjdf', 2, 58, 'M. van Ewijk']]</t>
         </is>
@@ -8759,6 +9129,11 @@
       </c>
       <c r="T95" t="inlineStr">
         <is>
+          <t>De Grolsch Veste</t>
+        </is>
+      </c>
+      <c r="U95" t="inlineStr">
+        <is>
           <t>[['Twente', '4tic29sox7m39fy1ztgv0jsiq', 1, 34, 'R. van Wolfswinkel'], ['Go Ahead Eagles', 'b79uipsy57y1jqpy07h4i5ovk', 2, 92, 'W. Willumsson']]</t>
         </is>
       </c>
@@ -8856,6 +9231,11 @@
       </c>
       <c r="T96" t="inlineStr">
         <is>
+          <t>Stadion Galgenwaard</t>
+        </is>
+      </c>
+      <c r="U96" t="inlineStr">
+        <is>
           <t>[['Groningen', 'cos9hxi16eitbcbthof7zrm4m', 1, 40, 'F. Krüger'], ['Utrecht', 'ccpscwdcm65czscrun048ecn5', 2, 62, 'T. Booth'], ['Utrecht', 'ccpscwdcm65czscrun048ecn5', 2, 84, 'S. van de Streek']]</t>
         </is>
       </c>
@@ -8948,6 +9328,11 @@
         </is>
       </c>
       <c r="T97" t="inlineStr">
+        <is>
+          <t>Kras Stadion</t>
+        </is>
+      </c>
+      <c r="U97" t="inlineStr">
         <is>
           <t>[['Feyenoord', '20vymiy7bo8wkyxai3ew494fz', 1, 16, 'Danilo'], ['Feyenoord', '20vymiy7bo8wkyxai3ew494fz', 1, 43, 'S. Szymański']]</t>
         </is>
@@ -9042,6 +9427,11 @@
         </is>
       </c>
       <c r="T98" t="inlineStr">
+        <is>
+          <t>Euroborg</t>
+        </is>
+      </c>
+      <c r="U98" t="inlineStr">
         <is>
           <t>[['Groningen', 'cos9hxi16eitbcbthof7zrm4m', 1, 45, 'R. Pepi'], ['Fortuna Sittard', '3ebril33e08ddzob4bhq8awsr', 2, 78, 'P. Gladon'], ['Fortuna Sittard', '3ebril33e08ddzob4bhq8awsr', 2, 84, 'P. Gladon'], ['Groningen', 'cos9hxi16eitbcbthof7zrm4m', 2, 91, 'F. Krüger'], ['Fortuna Sittard', '3ebril33e08ddzob4bhq8awsr', 2, 95, 'T. Noslin']]</t>
         </is>
@@ -9138,6 +9528,11 @@
         </is>
       </c>
       <c r="T99" t="inlineStr">
+        <is>
+          <t>Kras Stadion</t>
+        </is>
+      </c>
+      <c r="U99" t="inlineStr">
         <is>
           <t>[['Utrecht', 'ccpscwdcm65czscrun048ecn5', 1, 14, 'T. Booth'], ['Utrecht', 'ccpscwdcm65czscrun048ecn5', 2, 73, 'B. Dost'], ['Utrecht', 'ccpscwdcm65czscrun048ecn5', 2, 84, 'S. van de Streek'], ['Utrecht', 'ccpscwdcm65czscrun048ecn5', 2, 92, 'C. Bozdoğan']]</t>
         </is>
@@ -9237,6 +9632,11 @@
       </c>
       <c r="T100" t="inlineStr">
         <is>
+          <t>Abe Lenstra Stadion</t>
+        </is>
+      </c>
+      <c r="U100" t="inlineStr">
+        <is>
           <t>[['Cambuur', 'ears40cp6opsgvhsy0dgyszpd', 1, 10, 'J. Jacobs'], ['Heerenveen', '4vd2t5schmvvufrfib7f2vjdf', 1, 36, 'A. Sarr'], ['Heerenveen', '4vd2t5schmvvufrfib7f2vjdf', 2, 81, 'A. Tahiri']]</t>
         </is>
       </c>
@@ -9330,6 +9730,11 @@
         </is>
       </c>
       <c r="T101" t="inlineStr">
+        <is>
+          <t>Sparta-Stadion Het Kasteel</t>
+        </is>
+      </c>
+      <c r="U101" t="inlineStr">
         <is>
           <t>[['Twente', '4tic29sox7m39fy1ztgv0jsiq', 2, 63, 'S. Steijn'], ['Sparta Rotterdam', '89w5c6pw7vn0dxypi61tt0g4k', 2, 71, 'A. Verschueren']]</t>
         </is>
@@ -9432,6 +9837,11 @@
       </c>
       <c r="T102" t="inlineStr">
         <is>
+          <t>Goffertstadion</t>
+        </is>
+      </c>
+      <c r="U102" t="inlineStr">
+        <is>
           <t>[['RKC Waalwijk', 'ed5nwjz5za3oyi20nxzgqivmx', 1, 4, 'D. Van den Buijs'], ['NEC', '8iawijq7s9s6d85mjz8wdslki', 1, 38, 'L. Dimata'], ['NEC', '8iawijq7s9s6d85mjz8wdslki', 2, 50, 'S. El Karouani'], ['NEC', '8iawijq7s9s6d85mjz8wdslki', 2, 73, 'M. Mattsson'], ['NEC', '8iawijq7s9s6d85mjz8wdslki', 2, 78, 'Pedro Marques'], ['NEC', '8iawijq7s9s6d85mjz8wdslki', 2, 88, 'E. Tavşan'], ['NEC', '8iawijq7s9s6d85mjz8wdslki', 2, 92, 'Pedro Marques']]</t>
         </is>
       </c>
@@ -9532,6 +9942,11 @@
       </c>
       <c r="T103" t="inlineStr">
         <is>
+          <t>De Oude Meerdijk</t>
+        </is>
+      </c>
+      <c r="U103" t="inlineStr">
+        <is>
           <t>[['Emmen', '3t0vjqtxc8wpjzv82i3oi2ova', 1, 6, 'J. Veldmate'], ['Ajax', 'd0zdg647gvgc95xdtk1vpbkys', 1, 8, 'K. Taylor'], ['Ajax', 'd0zdg647gvgc95xdtk1vpbkys', 1, 21, 'K. Taylor'], ['Ajax', 'd0zdg647gvgc95xdtk1vpbkys', 1, 25, 'S. Bergwijn'], ['Emmen', '3t0vjqtxc8wpjzv82i3oi2ova', 2, 58, 'R. Živković'], ['Emmen', '3t0vjqtxc8wpjzv82i3oi2ova', 2, 84, 'M. Bouchouari']]</t>
         </is>
       </c>
@@ -9631,6 +10046,11 @@
         </is>
       </c>
       <c r="T104" t="inlineStr">
+        <is>
+          <t>De Adelaarshorst</t>
+        </is>
+      </c>
+      <c r="U104" t="inlineStr">
         <is>
           <t>[['Go Ahead Eagles', 'b79uipsy57y1jqpy07h4i5ovk', 1, 8, 'P. Rommens'], ['Go Ahead Eagles', 'b79uipsy57y1jqpy07h4i5ovk', 1, 20, 'P. Rommens'], ['Vitesse', '6hsriqr3ybvyg94w2k19oal50', 2, 49, 'M. Bero'], ['Vitesse', '6hsriqr3ybvyg94w2k19oal50', 2, 93, 'S. van Duivenbooden']]</t>
         </is>
@@ -9734,6 +10154,11 @@
       </c>
       <c r="T105" t="inlineStr">
         <is>
+          <t>Stadion Feijenoord</t>
+        </is>
+      </c>
+      <c r="U105" t="inlineStr">
+        <is>
           <t>[['Excelsior', 'dqk062lu0vm8epvytbm6r4mmf', 1, 4, 'K. Goudmijn'], ['Feyenoord', '20vymiy7bo8wkyxai3ew494fz', 1, 11, 'S. Szymański'], ['Feyenoord', '20vymiy7bo8wkyxai3ew494fz', 1, 20, 'O. Kökçü'], ['Feyenoord', '20vymiy7bo8wkyxai3ew494fz', 2, 50, 'S. Szymański'], ['Feyenoord', '20vymiy7bo8wkyxai3ew494fz', 2, 66, 'O. Kökçü'], ['Feyenoord', '20vymiy7bo8wkyxai3ew494fz', 2, 78, 'P. Wålemark']]</t>
         </is>
       </c>
@@ -9828,6 +10253,11 @@
         </is>
       </c>
       <c r="T106" t="inlineStr">
+        <is>
+          <t>Philips Stadion</t>
+        </is>
+      </c>
+      <c r="U106" t="inlineStr">
         <is>
           <t>[['AZ', '3kfktv64h7kg7zryax1wktr5r', 1, 18, 'V. Pavlidis']]</t>
         </is>
@@ -9929,6 +10359,11 @@
       </c>
       <c r="T107" t="inlineStr">
         <is>
+          <t>De Grolsch Veste</t>
+        </is>
+      </c>
+      <c r="U107" t="inlineStr">
+        <is>
           <t>[['Twente', '4tic29sox7m39fy1ztgv0jsiq', 1, 5, 'R. van Wolfswinkel'], ['Twente', '4tic29sox7m39fy1ztgv0jsiq', 2, 67, 'M. Sadílek']]</t>
         </is>
       </c>
@@ -10023,6 +10458,11 @@
       </c>
       <c r="T108" t="inlineStr">
         <is>
+          <t>Mandemakers Stadion</t>
+        </is>
+      </c>
+      <c r="U108" t="inlineStr">
+        <is>
           <t>[]</t>
         </is>
       </c>
@@ -10117,6 +10557,11 @@
       </c>
       <c r="T109" t="inlineStr">
         <is>
+          <t>AFAS Stadion</t>
+        </is>
+      </c>
+      <c r="U109" t="inlineStr">
+        <is>
           <t>[['AZ', '3kfktv64h7kg7zryax1wktr5r', 2, 77, 'V. Pavlidis'], ['Vitesse', '6hsriqr3ybvyg94w2k19oal50', 2, 87, 'M. Sankoh']]</t>
         </is>
       </c>
@@ -10209,6 +10654,11 @@
         </is>
       </c>
       <c r="T110" t="inlineStr">
+        <is>
+          <t>Fortuna Sittard Stadion</t>
+        </is>
+      </c>
+      <c r="U110" t="inlineStr">
         <is>
           <t>[['Go Ahead Eagles', 'b79uipsy57y1jqpy07h4i5ovk', 1, 21, 'B. Kuipers'], ['Go Ahead Eagles', 'b79uipsy57y1jqpy07h4i5ovk', 1, 44, 'B. Adekanye']]</t>
         </is>
@@ -10303,6 +10753,11 @@
         </is>
       </c>
       <c r="T111" t="inlineStr">
+        <is>
+          <t>Philips Stadion</t>
+        </is>
+      </c>
+      <c r="U111" t="inlineStr">
         <is>
           <t>[]</t>
         </is>
@@ -10400,6 +10855,11 @@
       </c>
       <c r="T112" t="inlineStr">
         <is>
+          <t>Stadion Galgenwaard</t>
+        </is>
+      </c>
+      <c r="U112" t="inlineStr">
+        <is>
           <t>[['Utrecht', 'ccpscwdcm65czscrun048ecn5', 1, 3, 'J. Toornstra'], ['Feyenoord', '20vymiy7bo8wkyxai3ew494fz', 2, 90, 'A. Jahanbakhsh']]</t>
         </is>
       </c>
@@ -10493,6 +10953,11 @@
         </is>
       </c>
       <c r="T113" t="inlineStr">
+        <is>
+          <t>Cambuur Stadion</t>
+        </is>
+      </c>
+      <c r="U113" t="inlineStr">
         <is>
           <t>[['Volendam', '6g9qrm72224jrk6tkxxxi8a9n', 1, 8, 'B. Ould-Chikh'], ['Volendam', '6g9qrm72224jrk6tkxxxi8a9n', 1, 9, 'R. Mühren'], ['Volendam', '6g9qrm72224jrk6tkxxxi8a9n', 2, 74, 'H. Veerman']]</t>
         </is>
@@ -10590,6 +11055,11 @@
       </c>
       <c r="T114" t="inlineStr">
         <is>
+          <t>Goffertstadion</t>
+        </is>
+      </c>
+      <c r="U114" t="inlineStr">
+        <is>
           <t>[['Ajax', 'd0zdg647gvgc95xdtk1vpbkys', 1, 38, 'D. Klaassen'], ['NEC', '8iawijq7s9s6d85mjz8wdslki', 2, 52, 'L. Dimata']]</t>
         </is>
       </c>
@@ -10684,6 +11154,11 @@
         </is>
       </c>
       <c r="T115" t="inlineStr">
+        <is>
+          <t>Van Donge &amp; De Roo Stadion</t>
+        </is>
+      </c>
+      <c r="U115" t="inlineStr">
         <is>
           <t>[['Excelsior', 'dqk062lu0vm8epvytbm6r4mmf', 2, 69, 'R. El Yaakoubi']]</t>
         </is>
@@ -10784,6 +11259,11 @@
       </c>
       <c r="T116" t="inlineStr">
         <is>
+          <t>Abe Lenstra Stadion</t>
+        </is>
+      </c>
+      <c r="U116" t="inlineStr">
+        <is>
           <t>[['AZ', '3kfktv64h7kg7zryax1wktr5r', 1, 33, 'D. de Wit'], ['AZ', '3kfktv64h7kg7zryax1wktr5r', 2, 46, 'T. Reijnders']]</t>
         </is>
       </c>
@@ -10877,6 +11357,11 @@
         </is>
       </c>
       <c r="T117" t="inlineStr">
+        <is>
+          <t>Euroborg</t>
+        </is>
+      </c>
+      <c r="U117" t="inlineStr">
         <is>
           <t>[['Feyenoord', '20vymiy7bo8wkyxai3ew494fz', 1, 19, 'Igor Paixão'], ['Feyenoord', '20vymiy7bo8wkyxai3ew494fz', 1, 30, 'O. Kökçü'], ['Feyenoord', '20vymiy7bo8wkyxai3ew494fz', 2, 91, 'S. Giménez']]</t>
         </is>
@@ -10972,6 +11457,11 @@
         </is>
       </c>
       <c r="T118" t="inlineStr">
+        <is>
+          <t>Sparta-Stadion Het Kasteel</t>
+        </is>
+      </c>
+      <c r="U118" t="inlineStr">
         <is>
           <t>[['Sparta Rotterdam', '89w5c6pw7vn0dxypi61tt0g4k', 2, 91, 'J. Kitolano']]</t>
         </is>
@@ -11072,6 +11562,11 @@
       </c>
       <c r="T119" t="inlineStr">
         <is>
+          <t>Johan Cruijff Arena</t>
+        </is>
+      </c>
+      <c r="U119" t="inlineStr">
+        <is>
           <t>[]</t>
         </is>
       </c>
@@ -11168,6 +11663,11 @@
       </c>
       <c r="T120" t="inlineStr">
         <is>
+          <t>Kras Stadion</t>
+        </is>
+      </c>
+      <c r="U120" t="inlineStr">
+        <is>
           <t>[['RKC Waalwijk', 'ed5nwjz5za3oyi20nxzgqivmx', 2, 63, 'M. Seuntjens'], ['Volendam', '6g9qrm72224jrk6tkxxxi8a9n', 2, 69, 'X. Mbuyamba'], ['Volendam', '6g9qrm72224jrk6tkxxxi8a9n', 2, 81, 'F. Da Silva']]</t>
         </is>
       </c>
@@ -11262,6 +11762,11 @@
         </is>
       </c>
       <c r="T121" t="inlineStr">
+        <is>
+          <t>GelreDome</t>
+        </is>
+      </c>
+      <c r="U121" t="inlineStr">
         <is>
           <t>[]</t>
         </is>
@@ -11361,6 +11866,11 @@
       </c>
       <c r="T122" t="inlineStr">
         <is>
+          <t>Fortuna Sittard Stadion</t>
+        </is>
+      </c>
+      <c r="U122" t="inlineStr">
+        <is>
           <t>[['Fortuna Sittard', '3ebril33e08ddzob4bhq8awsr', 1, 46, 'Iñigo Córdoba'], ['PSV', '24fvcruwqrqvqa3aonf8c3zuy', 2, 65, 'X. Simons'], ['PSV', '24fvcruwqrqvqa3aonf8c3zuy', 2, 76, 'I. Sangaré'], ['Fortuna Sittard', '3ebril33e08ddzob4bhq8awsr', 2, 99, 'B. Yılmaz']]</t>
         </is>
       </c>
@@ -11458,6 +11968,11 @@
       </c>
       <c r="T123" t="inlineStr">
         <is>
+          <t>De Adelaarshorst</t>
+        </is>
+      </c>
+      <c r="U123" t="inlineStr">
+        <is>
           <t>[['Go Ahead Eagles', 'b79uipsy57y1jqpy07h4i5ovk', 1, 3, 'W. Willumsson'], ['Go Ahead Eagles', 'b79uipsy57y1jqpy07h4i5ovk', 1, 10, 'B. Adekanye'], ['Utrecht', 'ccpscwdcm65czscrun048ecn5', 1, 13, 'S. van de Streek'], ['Go Ahead Eagles', 'b79uipsy57y1jqpy07h4i5ovk', 2, 90, 'S. Sow']]</t>
         </is>
       </c>
@@ -11555,6 +12070,11 @@
       </c>
       <c r="T124" t="inlineStr">
         <is>
+          <t>De Oude Meerdijk</t>
+        </is>
+      </c>
+      <c r="U124" t="inlineStr">
+        <is>
           <t>[]</t>
         </is>
       </c>
@@ -11651,6 +12171,11 @@
       </c>
       <c r="T125" t="inlineStr">
         <is>
+          <t>Van Donge &amp; De Roo Stadion</t>
+        </is>
+      </c>
+      <c r="U125" t="inlineStr">
+        <is>
           <t>[['Volendam', '6g9qrm72224jrk6tkxxxi8a9n', 1, 18, 'D. Mirani'], ['Excelsior', 'dqk062lu0vm8epvytbm6r4mmf', 2, 80, 'M. Azarkan']]</t>
         </is>
       </c>
@@ -11743,6 +12268,11 @@
         </is>
       </c>
       <c r="T126" t="inlineStr">
+        <is>
+          <t>Goffertstadion</t>
+        </is>
+      </c>
+      <c r="U126" t="inlineStr">
         <is>
           <t>[['NEC', '8iawijq7s9s6d85mjz8wdslki', 1, 12, 'L. Dimata'], ['NEC', '8iawijq7s9s6d85mjz8wdslki', 1, 35, 'L. Dimata'], ['Emmen', '3t0vjqtxc8wpjzv82i3oi2ova', 1, 44, 'R. Živković'], ['NEC', '8iawijq7s9s6d85mjz8wdslki', 2, 52, 'I. Cissoko']]</t>
         </is>
@@ -11838,6 +12368,11 @@
         </is>
       </c>
       <c r="T127" t="inlineStr">
+        <is>
+          <t>Cambuur Stadion</t>
+        </is>
+      </c>
+      <c r="U127" t="inlineStr">
         <is>
           <t>[['Sparta Rotterdam', '89w5c6pw7vn0dxypi61tt0g4k', 1, 9, 'T. Lauritsen'], ['Sparta Rotterdam', '89w5c6pw7vn0dxypi61tt0g4k', 1, 18, 'K. Saito'], ['Sparta Rotterdam', '89w5c6pw7vn0dxypi61tt0g4k', 2, 51, 'V. van Crooij']]</t>
         </is>
@@ -11938,6 +12473,11 @@
       </c>
       <c r="T128" t="inlineStr">
         <is>
+          <t>Philips Stadion</t>
+        </is>
+      </c>
+      <c r="U128" t="inlineStr">
+        <is>
           <t>[['PSV', '24fvcruwqrqvqa3aonf8c3zuy', 2, 48, 'G. Til']]</t>
         </is>
       </c>
@@ -12036,6 +12576,11 @@
       </c>
       <c r="T129" t="inlineStr">
         <is>
+          <t>Mandemakers Stadion</t>
+        </is>
+      </c>
+      <c r="U129" t="inlineStr">
+        <is>
           <t>[['RKC Waalwijk', 'ed5nwjz5za3oyi20nxzgqivmx', 1, 24, 'M. Seuntjens'], ['Go Ahead Eagles', 'b79uipsy57y1jqpy07h4i5ovk', 1, 46, 'José Fontán'], ['RKC Waalwijk', 'ed5nwjz5za3oyi20nxzgqivmx', 2, 71, 'M. Kramer'], ['RKC Waalwijk', 'ed5nwjz5za3oyi20nxzgqivmx', 2, 78, 'Y. Oukili']]</t>
         </is>
       </c>
@@ -12133,6 +12678,11 @@
       </c>
       <c r="T130" t="inlineStr">
         <is>
+          <t>Abe Lenstra Stadion</t>
+        </is>
+      </c>
+      <c r="U130" t="inlineStr">
+        <is>
           <t>[['Heerenveen', '4vd2t5schmvvufrfib7f2vjdf', 1, 5, 'A. Sarr'], ['Groningen', 'cos9hxi16eitbcbthof7zrm4m', 1, 40, 'F. Krüger'], ['Heerenveen', '4vd2t5schmvvufrfib7f2vjdf', 2, 81, 'P. van Amersfoort'], ['Heerenveen', '4vd2t5schmvvufrfib7f2vjdf', 2, 82, 'A. Sarr']]</t>
         </is>
       </c>
@@ -12224,6 +12774,11 @@
         </is>
       </c>
       <c r="T131" t="inlineStr">
+        <is>
+          <t>De Grolsch Veste</t>
+        </is>
+      </c>
+      <c r="U131" t="inlineStr">
         <is>
           <t>[['Twente', '4tic29sox7m39fy1ztgv0jsiq', 1, 46, 'V. Černý'], ['Twente', '4tic29sox7m39fy1ztgv0jsiq', 2, 64, 'V. Misidjan']]</t>
         </is>
@@ -12321,6 +12876,11 @@
       </c>
       <c r="T132" t="inlineStr">
         <is>
+          <t>Stadion Feijenoord</t>
+        </is>
+      </c>
+      <c r="U132" t="inlineStr">
+        <is>
           <t>[['Feyenoord', '20vymiy7bo8wkyxai3ew494fz', 1, 34, 'Igor Paixão'], ['Ajax', 'd0zdg647gvgc95xdtk1vpbkys', 2, 71, 'D. Klaassen']]</t>
         </is>
       </c>
@@ -12414,6 +12974,11 @@
         </is>
       </c>
       <c r="T133" t="inlineStr">
+        <is>
+          <t>AFAS Stadion</t>
+        </is>
+      </c>
+      <c r="U133" t="inlineStr">
         <is>
           <t>[['AZ', '3kfktv64h7kg7zryax1wktr5r', 1, 4, 'D. de Wit'], ['Fortuna Sittard', '3ebril33e08ddzob4bhq8awsr', 1, 11, 'B. Yılmaz'], ['Fortuna Sittard', '3ebril33e08ddzob4bhq8awsr', 1, 24, 'Ximo Navarro'], ['AZ', '3kfktv64h7kg7zryax1wktr5r', 2, 56, 'V. Pavlidis']]</t>
         </is>
@@ -12518,6 +13083,11 @@
       </c>
       <c r="T134" t="inlineStr">
         <is>
+          <t>De Oude Meerdijk</t>
+        </is>
+      </c>
+      <c r="U134" t="inlineStr">
+        <is>
           <t>[['Emmen', '3t0vjqtxc8wpjzv82i3oi2ova', 1, 24, 'L. Bernadou']]</t>
         </is>
       </c>
@@ -12611,6 +13181,11 @@
         </is>
       </c>
       <c r="T135" t="inlineStr">
+        <is>
+          <t>Sparta-Stadion Het Kasteel</t>
+        </is>
+      </c>
+      <c r="U135" t="inlineStr">
         <is>
           <t>[]</t>
         </is>
@@ -12706,6 +13281,11 @@
         </is>
       </c>
       <c r="T136" t="inlineStr">
+        <is>
+          <t>De Adelaarshorst</t>
+        </is>
+      </c>
+      <c r="U136" t="inlineStr">
         <is>
           <t>[['AZ', '3kfktv64h7kg7zryax1wktr5r', 1, 38, 'V. Pavlidis'], ['AZ', '3kfktv64h7kg7zryax1wktr5r', 2, 57, 'D. Mihailovic'], ['AZ', '3kfktv64h7kg7zryax1wktr5r', 2, 87, 'Y. Sugawara'], ['Go Ahead Eagles', 'b79uipsy57y1jqpy07h4i5ovk', 2, 92, 'W. Willumsson'], ['AZ', '3kfktv64h7kg7zryax1wktr5r', 2, 95, 'Z. Buurmeester']]</t>
         </is>
@@ -12807,6 +13387,11 @@
       </c>
       <c r="T137" t="inlineStr">
         <is>
+          <t>GelreDome</t>
+        </is>
+      </c>
+      <c r="U137" t="inlineStr">
+        <is>
           <t>[['Twente', '4tic29sox7m39fy1ztgv0jsiq', 1, 33, 'R. van Wolfswinkel'], ['Vitesse', '6hsriqr3ybvyg94w2k19oal50', 1, 44, 'G. Vidović'], ['Vitesse', '6hsriqr3ybvyg94w2k19oal50', 2, 52, 'M. Bero'], ['Twente', '4tic29sox7m39fy1ztgv0jsiq', 2, 59, 'V. Černý']]</t>
         </is>
       </c>
@@ -12902,6 +13487,11 @@
       </c>
       <c r="T138" t="inlineStr">
         <is>
+          <t>Fortuna Sittard Stadion</t>
+        </is>
+      </c>
+      <c r="U138" t="inlineStr">
+        <is>
           <t>[['Fortuna Sittard', '3ebril33e08ddzob4bhq8awsr', 2, 58, 'Úmaro Embaló'], ['Fortuna Sittard', '3ebril33e08ddzob4bhq8awsr', 2, 98, 'B. Yılmaz']]</t>
         </is>
       </c>
@@ -12995,6 +13585,11 @@
         </is>
       </c>
       <c r="T139" t="inlineStr">
+        <is>
+          <t>Stadion Galgenwaard</t>
+        </is>
+      </c>
+      <c r="U139" t="inlineStr">
         <is>
           <t>[['Utrecht', 'ccpscwdcm65czscrun048ecn5', 1, 6, 'T. Douvikas']]</t>
         </is>
@@ -13094,6 +13689,11 @@
       </c>
       <c r="T140" t="inlineStr">
         <is>
+          <t>Stadion Feijenoord</t>
+        </is>
+      </c>
+      <c r="U140" t="inlineStr">
+        <is>
           <t>[['Feyenoord', '20vymiy7bo8wkyxai3ew494fz', 1, 9, 'J. Dilrosun'], ['Feyenoord', '20vymiy7bo8wkyxai3ew494fz', 1, 48, 'O. Kökçü']]</t>
         </is>
       </c>
@@ -13189,6 +13789,11 @@
         </is>
       </c>
       <c r="T141" t="inlineStr">
+        <is>
+          <t>Euroborg</t>
+        </is>
+      </c>
+      <c r="U141" t="inlineStr">
         <is>
           <t>[['Cambuur', 'ears40cp6opsgvhsy0dgyszpd', 2, 77, 'D. van Kaam']]</t>
         </is>
@@ -13291,6 +13896,11 @@
       </c>
       <c r="T142" t="inlineStr">
         <is>
+          <t>Johan Cruijff Arena</t>
+        </is>
+      </c>
+      <c r="U142" t="inlineStr">
+        <is>
           <t>[['Volendam', '6g9qrm72224jrk6tkxxxi8a9n', 2, 59, 'D. Mirani'], ['Ajax', 'd0zdg647gvgc95xdtk1vpbkys', 2, 80, 'M. Kudus']]</t>
         </is>
       </c>
@@ -13391,6 +14001,11 @@
         </is>
       </c>
       <c r="T143" t="inlineStr">
+        <is>
+          <t>Mandemakers Stadion</t>
+        </is>
+      </c>
+      <c r="U143" t="inlineStr">
         <is>
           <t>[['RKC Waalwijk', 'ed5nwjz5za3oyi20nxzgqivmx', 1, 3, 'M. Kramer'], ['RKC Waalwijk', 'ed5nwjz5za3oyi20nxzgqivmx', 1, 28, 'J. Lelieveld']]</t>
         </is>
@@ -13496,6 +14111,11 @@
       </c>
       <c r="T144" t="inlineStr">
         <is>
+          <t>Philips Stadion</t>
+        </is>
+      </c>
+      <c r="U144" t="inlineStr">
+        <is>
           <t>[['PSV', '24fvcruwqrqvqa3aonf8c3zuy', 1, 14, 'J. Veerman'], ['PSV', '24fvcruwqrqvqa3aonf8c3zuy', 2, 64, 'A. El Ghazi']]</t>
         </is>
       </c>
@@ -13590,6 +14210,11 @@
         </is>
       </c>
       <c r="T145" t="inlineStr">
+        <is>
+          <t>Goffertstadion</t>
+        </is>
+      </c>
+      <c r="U145" t="inlineStr">
         <is>
           <t>[['Sparta Rotterdam', '89w5c6pw7vn0dxypi61tt0g4k', 2, 58, 'A. Verschueren'], ['NEC', '8iawijq7s9s6d85mjz8wdslki', 2, 80, 'Pedro Marques']]</t>
         </is>
@@ -13688,6 +14313,11 @@
         </is>
       </c>
       <c r="T146" t="inlineStr">
+        <is>
+          <t>Abe Lenstra Stadion</t>
+        </is>
+      </c>
+      <c r="U146" t="inlineStr">
         <is>
           <t>[['Heerenveen', '4vd2t5schmvvufrfib7f2vjdf', 1, 21, 'P. van Amersfoort'], ['Vitesse', '6hsriqr3ybvyg94w2k19oal50', 1, 32, 'B. Białek'], ['Vitesse', '6hsriqr3ybvyg94w2k19oal50', 1, 45, 'G. Vidović'], ['Vitesse', '6hsriqr3ybvyg94w2k19oal50', 2, 47, 'M. Manhoef']]</t>
         </is>
@@ -13791,6 +14421,11 @@
       </c>
       <c r="T147" t="inlineStr">
         <is>
+          <t>AFAS Stadion</t>
+        </is>
+      </c>
+      <c r="U147" t="inlineStr">
+        <is>
           <t>[['Utrecht', 'ccpscwdcm65czscrun048ecn5', 1, 12, 'T. Douvikas'], ['Utrecht', 'ccpscwdcm65czscrun048ecn5', 1, 16, 'T. Douvikas'], ['AZ', '3kfktv64h7kg7zryax1wktr5r', 1, 20, 'M. Dekker'], ['AZ', '3kfktv64h7kg7zryax1wktr5r', 1, 30, 'V. Pavlidis'], ['AZ', '3kfktv64h7kg7zryax1wktr5r', 1, 34, 'V. Pavlidis'], ['Utrecht', 'ccpscwdcm65czscrun048ecn5', 1, 41, 'N. Viergever'], ['Utrecht', 'ccpscwdcm65czscrun048ecn5', 2, 65, 'T. Douvikas'], ['AZ', '3kfktv64h7kg7zryax1wktr5r', 2, 70, 'M. de Wit'], ['AZ', '3kfktv64h7kg7zryax1wktr5r', 2, 78, 'V. Pavlidis'], ['Utrecht', 'ccpscwdcm65czscrun048ecn5', 2, 80, 'S. van de Streek']]</t>
         </is>
       </c>
@@ -13890,6 +14525,11 @@
       </c>
       <c r="T148" t="inlineStr">
         <is>
+          <t>De Grolsch Veste</t>
+        </is>
+      </c>
+      <c r="U148" t="inlineStr">
+        <is>
           <t>[['Feyenoord', '20vymiy7bo8wkyxai3ew494fz', 1, 30, 'S. Giménez'], ['Twente', '4tic29sox7m39fy1ztgv0jsiq', 2, 68, 'J. Brenet']]</t>
         </is>
       </c>
@@ -13985,6 +14625,11 @@
         </is>
       </c>
       <c r="T149" t="inlineStr">
+        <is>
+          <t>Van Donge &amp; De Roo Stadion</t>
+        </is>
+      </c>
+      <c r="U149" t="inlineStr">
         <is>
           <t>[['Ajax', 'd0zdg647gvgc95xdtk1vpbkys', 1, 15, 'D. Tadić'], ['Excelsior', 'dqk062lu0vm8epvytbm6r4mmf', 1, 36, 'R. El Yaakoubi'], ['Ajax', 'd0zdg647gvgc95xdtk1vpbkys', 1, 45, 'D. Klaassen'], ['Ajax', 'd0zdg647gvgc95xdtk1vpbkys', 2, 61, 'M. Kudus'], ['Ajax', 'd0zdg647gvgc95xdtk1vpbkys', 2, 83, 'D. Rensch']]</t>
         </is>
@@ -14084,6 +14729,11 @@
         </is>
       </c>
       <c r="T150" t="inlineStr">
+        <is>
+          <t>Kras Stadion</t>
+        </is>
+      </c>
+      <c r="U150" t="inlineStr">
         <is>
           <t>[['Volendam', '6g9qrm72224jrk6tkxxxi8a9n', 1, 21, 'G. Oristanio'], ['Groningen', 'cos9hxi16eitbcbthof7zrm4m', 2, 50, 'J. Hove'], ['Volendam', '6g9qrm72224jrk6tkxxxi8a9n', 2, 55, 'C. Twigt'], ['Groningen', 'cos9hxi16eitbcbthof7zrm4m', 2, 73, 'R. Pepi'], ['Volendam', '6g9qrm72224jrk6tkxxxi8a9n', 2, 78, 'R. Mühren']]</t>
         </is>
@@ -14185,6 +14835,11 @@
       </c>
       <c r="T151" t="inlineStr">
         <is>
+          <t>Cambuur Stadion</t>
+        </is>
+      </c>
+      <c r="U151" t="inlineStr">
+        <is>
           <t>[['Cambuur', 'ears40cp6opsgvhsy0dgyszpd', 1, 31, 'M. Hoedemakers'], ['Fortuna Sittard', '3ebril33e08ddzob4bhq8awsr', 2, 75, 'B. Yılmaz'], ['Fortuna Sittard', '3ebril33e08ddzob4bhq8awsr', 2, 84, 'Iñigo Córdoba']]</t>
         </is>
       </c>
@@ -14277,6 +14932,11 @@
         </is>
       </c>
       <c r="T152" t="inlineStr">
+        <is>
+          <t>Fortuna Sittard Stadion</t>
+        </is>
+      </c>
+      <c r="U152" t="inlineStr">
         <is>
           <t>[]</t>
         </is>
@@ -14376,6 +15036,11 @@
       </c>
       <c r="T153" t="inlineStr">
         <is>
+          <t>Kras Stadion</t>
+        </is>
+      </c>
+      <c r="U153" t="inlineStr">
+        <is>
           <t>[['Volendam', '6g9qrm72224jrk6tkxxxi8a9n', 2, 62, 'X. Mbuyamba'], ['AZ', '3kfktv64h7kg7zryax1wktr5r', 2, 83, 'J. Odgaard']]</t>
         </is>
       </c>
@@ -14474,6 +15139,11 @@
       </c>
       <c r="T154" t="inlineStr">
         <is>
+          <t>Stadion Galgenwaard</t>
+        </is>
+      </c>
+      <c r="U154" t="inlineStr">
+        <is>
           <t>[['Utrecht', 'ccpscwdcm65czscrun048ecn5', 2, 69, 'T. Douvikas']]</t>
         </is>
       </c>
@@ -14568,6 +15238,11 @@
       </c>
       <c r="T155" t="inlineStr">
         <is>
+          <t>De Oude Meerdijk</t>
+        </is>
+      </c>
+      <c r="U155" t="inlineStr">
+        <is>
           <t>[['Vitesse', '6hsriqr3ybvyg94w2k19oal50', 1, 33, 'M. Manhoef'], ['Vitesse', '6hsriqr3ybvyg94w2k19oal50', 1, 38, 'C. Arcus'], ['Emmen', '3t0vjqtxc8wpjzv82i3oi2ova', 1, 43, 'J. Assehnoun'], ['Vitesse', '6hsriqr3ybvyg94w2k19oal50', 2, 87, 'D. Oroz']]</t>
         </is>
       </c>
@@ -14661,6 +15336,11 @@
         </is>
       </c>
       <c r="T156" t="inlineStr">
+        <is>
+          <t>Van Donge &amp; De Roo Stadion</t>
+        </is>
+      </c>
+      <c r="U156" t="inlineStr">
         <is>
           <t>[]</t>
         </is>
@@ -14758,6 +15438,11 @@
       </c>
       <c r="T157" t="inlineStr">
         <is>
+          <t>Cambuur Stadion</t>
+        </is>
+      </c>
+      <c r="U157" t="inlineStr">
+        <is>
           <t>[['Ajax', 'd0zdg647gvgc95xdtk1vpbkys', 1, 16, 'D. Tadić'], ['Ajax', 'd0zdg647gvgc95xdtk1vpbkys', 1, 36, 'S. Berghuis'], ['Ajax', 'd0zdg647gvgc95xdtk1vpbkys', 2, 64, 'S. Berghuis'], ['Ajax', 'd0zdg647gvgc95xdtk1vpbkys', 2, 79, 'B. Brobbey'], ['Ajax', 'd0zdg647gvgc95xdtk1vpbkys', 2, 93, 'B. Brobbey']]</t>
         </is>
       </c>
@@ -14850,6 +15535,11 @@
         </is>
       </c>
       <c r="T158" t="inlineStr">
+        <is>
+          <t>De Adelaarshorst</t>
+        </is>
+      </c>
+      <c r="U158" t="inlineStr">
         <is>
           <t>[['Go Ahead Eagles', 'b79uipsy57y1jqpy07h4i5ovk', 1, 35, 'F. Stokkers']]</t>
         </is>
@@ -14951,6 +15641,11 @@
       </c>
       <c r="T159" t="inlineStr">
         <is>
+          <t>Stadion Feijenoord</t>
+        </is>
+      </c>
+      <c r="U159" t="inlineStr">
+        <is>
           <t>[['PSV', '24fvcruwqrqvqa3aonf8c3zuy', 1, 8, 'A. El Ghazi'], ['PSV', '24fvcruwqrqvqa3aonf8c3zuy', 2, 68, 'T. Hazard'], ['Feyenoord', '20vymiy7bo8wkyxai3ew494fz', 2, 81, 'A. Jahanbakhsh'], ['Feyenoord', '20vymiy7bo8wkyxai3ew494fz', 2, 96, 'A. Jahanbakhsh']]</t>
         </is>
       </c>
@@ -15050,6 +15745,11 @@
       </c>
       <c r="T160" t="inlineStr">
         <is>
+          <t>Euroborg</t>
+        </is>
+      </c>
+      <c r="U160" t="inlineStr">
+        <is>
           <t>[['Twente', '4tic29sox7m39fy1ztgv0jsiq', 1, 5, 'S. Steijn'], ['Groningen', 'cos9hxi16eitbcbthof7zrm4m', 2, 69, 'O. Antman']]</t>
         </is>
       </c>
@@ -15147,6 +15847,11 @@
       </c>
       <c r="T161" t="inlineStr">
         <is>
+          <t>Abe Lenstra Stadion</t>
+        </is>
+      </c>
+      <c r="U161" t="inlineStr">
+        <is>
           <t>[['Feyenoord', '20vymiy7bo8wkyxai3ew494fz', 1, 22, 'L. Geertruida'], ['Feyenoord', '20vymiy7bo8wkyxai3ew494fz', 1, 34, 'S. Giménez'], ['Heerenveen', '4vd2t5schmvvufrfib7f2vjdf', 2, 75, 'S. van Ottele']]</t>
         </is>
       </c>
@@ -15244,6 +15949,11 @@
       </c>
       <c r="T162" t="inlineStr">
         <is>
+          <t>AFAS Stadion</t>
+        </is>
+      </c>
+      <c r="U162" t="inlineStr">
+        <is>
           <t>[['AZ', '3kfktv64h7kg7zryax1wktr5r', 1, 20, 'S. Mijnans'], ['AZ', '3kfktv64h7kg7zryax1wktr5r', 1, 27, 'J. Karlsson'], ['AZ', '3kfktv64h7kg7zryax1wktr5r', 1, 30, 'S. Mijnans'], ['AZ', '3kfktv64h7kg7zryax1wktr5r', 1, 35, 'J. Odgaard'], ['AZ', '3kfktv64h7kg7zryax1wktr5r', 1, 38, 'V. Pavlidis']]</t>
         </is>
       </c>
@@ -15340,6 +16050,11 @@
       </c>
       <c r="T163" t="inlineStr">
         <is>
+          <t>Johan Cruijff Arena</t>
+        </is>
+      </c>
+      <c r="U163" t="inlineStr">
+        <is>
           <t>[['RKC Waalwijk', 'ed5nwjz5za3oyi20nxzgqivmx', 1, 17, 'M. Seuntjens'], ['Ajax', 'd0zdg647gvgc95xdtk1vpbkys', 2, 50, 'B. Brobbey'], ['Ajax', 'd0zdg647gvgc95xdtk1vpbkys', 2, 78, 'J. Timber'], ['Ajax', 'd0zdg647gvgc95xdtk1vpbkys', 2, 81, 'M. Kudus']]</t>
         </is>
       </c>
@@ -15436,6 +16151,11 @@
       </c>
       <c r="T164" t="inlineStr">
         <is>
+          <t>De Oude Meerdijk</t>
+        </is>
+      </c>
+      <c r="U164" t="inlineStr">
+        <is>
           <t>[['Fortuna Sittard', '3ebril33e08ddzob4bhq8awsr', 2, 76, 'O. Özyakup']]</t>
         </is>
       </c>
@@ -15527,6 +16247,11 @@
         </is>
       </c>
       <c r="T165" t="inlineStr">
+        <is>
+          <t>De Grolsch Veste</t>
+        </is>
+      </c>
+      <c r="U165" t="inlineStr">
         <is>
           <t>[['Twente', '4tic29sox7m39fy1ztgv0jsiq', 1, 16, 'J. Brenet'], ['Twente', '4tic29sox7m39fy1ztgv0jsiq', 1, 17, 'V. Černý'], ['Twente', '4tic29sox7m39fy1ztgv0jsiq', 1, 20, 'M. Hilgers']]</t>
         </is>
@@ -15621,6 +16346,11 @@
         </is>
       </c>
       <c r="T166" t="inlineStr">
+        <is>
+          <t>Goffertstadion</t>
+        </is>
+      </c>
+      <c r="U166" t="inlineStr">
         <is>
           <t>[]</t>
         </is>
@@ -15716,6 +16446,11 @@
         </is>
       </c>
       <c r="T167" t="inlineStr">
+        <is>
+          <t>Philips Stadion</t>
+        </is>
+      </c>
+      <c r="U167" t="inlineStr">
         <is>
           <t>[['PSV', '24fvcruwqrqvqa3aonf8c3zuy', 1, 27, 'L. de Jong'], ['PSV', '24fvcruwqrqvqa3aonf8c3zuy', 2, 46, 'X. Simons'], ['PSV', '24fvcruwqrqvqa3aonf8c3zuy', 2, 69, 'J. Branthwaite'], ['PSV', '24fvcruwqrqvqa3aonf8c3zuy', 2, 73, 'J. Bakayoko'], ['PSV', '24fvcruwqrqvqa3aonf8c3zuy', 2, 84, 'Fábio Silva'], ['PSV', '24fvcruwqrqvqa3aonf8c3zuy', 2, 88, 'G. Til']]</t>
         </is>
@@ -15813,6 +16548,11 @@
       </c>
       <c r="T168" t="inlineStr">
         <is>
+          <t>Sparta-Stadion Het Kasteel</t>
+        </is>
+      </c>
+      <c r="U168" t="inlineStr">
+        <is>
           <t>[['Sparta Rotterdam', '89w5c6pw7vn0dxypi61tt0g4k', 1, 4, 'V. van Crooij'], ['Go Ahead Eagles', 'b79uipsy57y1jqpy07h4i5ovk', 2, 53, 'F. Stokkers'], ['Sparta Rotterdam', '89w5c6pw7vn0dxypi61tt0g4k', 2, 58, 'T. Lauritsen']]</t>
         </is>
       </c>
@@ -15905,6 +16645,11 @@
         </is>
       </c>
       <c r="T169" t="inlineStr">
+        <is>
+          <t>GelreDome</t>
+        </is>
+      </c>
+      <c r="U169" t="inlineStr">
         <is>
           <t>[['Vitesse', '6hsriqr3ybvyg94w2k19oal50', 2, 63, 'M. Manhoef'], ['Vitesse', '6hsriqr3ybvyg94w2k19oal50', 2, 94, 'M. Wittek']]</t>
         </is>
@@ -16000,6 +16745,11 @@
         </is>
       </c>
       <c r="T170" t="inlineStr">
+        <is>
+          <t>Euroborg</t>
+        </is>
+      </c>
+      <c r="U170" t="inlineStr">
         <is>
           <t>[['Groningen', 'cos9hxi16eitbcbthof7zrm4m', 1, 12, 'R. Pepi'], ['Emmen', '3t0vjqtxc8wpjzv82i3oi2ova', 1, 14, 'M. Araujo']]</t>
         </is>
@@ -16098,6 +16848,11 @@
       </c>
       <c r="T171" t="inlineStr">
         <is>
+          <t>Stadion Galgenwaard</t>
+        </is>
+      </c>
+      <c r="U171" t="inlineStr">
+        <is>
           <t>[['Utrecht', 'ccpscwdcm65czscrun048ecn5', 1, 33, 'O. Boussaid'], ['PSV', '24fvcruwqrqvqa3aonf8c3zuy', 1, 41, 'J. Bakayoko'], ['PSV', '24fvcruwqrqvqa3aonf8c3zuy', 2, 57, 'L. de Jong'], ['Utrecht', 'ccpscwdcm65czscrun048ecn5', 2, 60, 'S. van de Streek']]</t>
         </is>
       </c>
@@ -16192,6 +16947,11 @@
         </is>
       </c>
       <c r="T172" t="inlineStr">
+        <is>
+          <t>Johan Cruijff Arena</t>
+        </is>
+      </c>
+      <c r="U172" t="inlineStr">
         <is>
           <t>[['Ajax', 'd0zdg647gvgc95xdtk1vpbkys', 1, 6, 'D. Tadić'], ['Ajax', 'd0zdg647gvgc95xdtk1vpbkys', 1, 27, 'K. Taylor'], ['Ajax', 'd0zdg647gvgc95xdtk1vpbkys', 2, 64, 'D. Tadić'], ['Ajax', 'd0zdg647gvgc95xdtk1vpbkys', 2, 84, 'M. Kudus']]</t>
         </is>
@@ -16290,6 +17050,11 @@
       </c>
       <c r="T173" t="inlineStr">
         <is>
+          <t>Van Donge &amp; De Roo Stadion</t>
+        </is>
+      </c>
+      <c r="U173" t="inlineStr">
+        <is>
           <t>[['NEC', '8iawijq7s9s6d85mjz8wdslki', 1, 44, 'M. Mattsson'], ['NEC', '8iawijq7s9s6d85mjz8wdslki', 2, 73, 'S. El Karouani'], ['NEC', '8iawijq7s9s6d85mjz8wdslki', 2, 85, 'A. Musaba']]</t>
         </is>
       </c>
@@ -16386,6 +17151,11 @@
       </c>
       <c r="T174" t="inlineStr">
         <is>
+          <t>Cambuur Stadion</t>
+        </is>
+      </c>
+      <c r="U174" t="inlineStr">
+        <is>
           <t>[['Cambuur', 'ears40cp6opsgvhsy0dgyszpd', 1, 1, 'B. Johnsen'], ['Heerenveen', '4vd2t5schmvvufrfib7f2vjdf', 1, 22, 'O. Sahraoui'], ['Heerenveen', '4vd2t5schmvvufrfib7f2vjdf', 2, 65, 'M. van Ewijk']]</t>
         </is>
       </c>
@@ -16482,6 +17252,11 @@
       </c>
       <c r="T175" t="inlineStr">
         <is>
+          <t>Mandemakers Stadion</t>
+        </is>
+      </c>
+      <c r="U175" t="inlineStr">
+        <is>
           <t>[['Fortuna Sittard', '3ebril33e08ddzob4bhq8awsr', 2, 49, 'B. Yılmaz'], ['RKC Waalwijk', 'ed5nwjz5za3oyi20nxzgqivmx', 2, 76, 'M. Kramer'], ['RKC Waalwijk', 'ed5nwjz5za3oyi20nxzgqivmx', 2, 86, 'Julen Lobete'], ['RKC Waalwijk', 'ed5nwjz5za3oyi20nxzgqivmx', 2, 90, 'F. Jozefzoon']]</t>
         </is>
       </c>
@@ -16575,6 +17350,11 @@
         </is>
       </c>
       <c r="T176" t="inlineStr">
+        <is>
+          <t>De Adelaarshorst</t>
+        </is>
+      </c>
+      <c r="U176" t="inlineStr">
         <is>
           <t>[['Go Ahead Eagles', 'b79uipsy57y1jqpy07h4i5ovk', 1, 6, 'P. Rommens'], ['Go Ahead Eagles', 'b79uipsy57y1jqpy07h4i5ovk', 1, 16, 'I. Lidberg']]</t>
         </is>
@@ -16672,6 +17452,11 @@
         </is>
       </c>
       <c r="T177" t="inlineStr">
+        <is>
+          <t>Stadion Feijenoord</t>
+        </is>
+      </c>
+      <c r="U177" t="inlineStr">
         <is>
           <t>[['Feyenoord', '20vymiy7bo8wkyxai3ew494fz', 1, 17, 'J. Dilrosun'], ['Feyenoord', '20vymiy7bo8wkyxai3ew494fz', 1, 47, 'A. Jahanbakhsh'], ['Feyenoord', '20vymiy7bo8wkyxai3ew494fz', 2, 90, 'M. Pedersen']]</t>
         </is>
@@ -16770,6 +17555,11 @@
         </is>
       </c>
       <c r="T178" t="inlineStr">
+        <is>
+          <t>Kras Stadion</t>
+        </is>
+      </c>
+      <c r="U178" t="inlineStr">
         <is>
           <t>[['Volendam', '6g9qrm72224jrk6tkxxxi8a9n', 1, 12, 'D. van Mieghem'], ['Volendam', '6g9qrm72224jrk6tkxxxi8a9n', 2, 68, 'D. van Mieghem']]</t>
         </is>
@@ -16872,6 +17662,11 @@
       </c>
       <c r="T179" t="inlineStr">
         <is>
+          <t>AFAS Stadion</t>
+        </is>
+      </c>
+      <c r="U179" t="inlineStr">
+        <is>
           <t>[['AZ', '3kfktv64h7kg7zryax1wktr5r', 1, 40, 'V. Pavlidis'], ['AZ', '3kfktv64h7kg7zryax1wktr5r', 2, 73, 'W. Goes'], ['Cambuur', 'ears40cp6opsgvhsy0dgyszpd', 2, 85, 'B. Johnsen']]</t>
         </is>
       </c>
@@ -16970,6 +17765,11 @@
       </c>
       <c r="T180" t="inlineStr">
         <is>
+          <t>Sparta-Stadion Het Kasteel</t>
+        </is>
+      </c>
+      <c r="U180" t="inlineStr">
+        <is>
           <t>[['Utrecht', 'ccpscwdcm65czscrun048ecn5', 2, 74, 'V. Jensen'], ['Utrecht', 'ccpscwdcm65czscrun048ecn5', 2, 88, 'O. Boussaid'], ['Utrecht', 'ccpscwdcm65czscrun048ecn5', 2, 90, 'A. Descotte']]</t>
         </is>
       </c>
@@ -17064,6 +17864,11 @@
         </is>
       </c>
       <c r="T181" t="inlineStr">
+        <is>
+          <t>Philips Stadion</t>
+        </is>
+      </c>
+      <c r="U181" t="inlineStr">
         <is>
           <t>[['PSV', '24fvcruwqrqvqa3aonf8c3zuy', 1, 9, 'Fábio Silva'], ['Twente', '4tic29sox7m39fy1ztgv0jsiq', 2, 47, 'V. Misidjan'], ['PSV', '24fvcruwqrqvqa3aonf8c3zuy', 2, 57, 'L. de Jong'], ['PSV', '24fvcruwqrqvqa3aonf8c3zuy', 2, 74, 'X. Simons']]</t>
         </is>
@@ -17160,6 +17965,11 @@
         </is>
       </c>
       <c r="T182" t="inlineStr">
+        <is>
+          <t>GelreDome</t>
+        </is>
+      </c>
+      <c r="U182" t="inlineStr">
         <is>
           <t>[['Vitesse', '6hsriqr3ybvyg94w2k19oal50', 1, 30, 'M. van Ginkel'], ['Ajax', 'd0zdg647gvgc95xdtk1vpbkys', 1, 32, 'D. Klaassen'], ['Ajax', 'd0zdg647gvgc95xdtk1vpbkys', 2, 54, 'E. Álvarez']]</t>
         </is>
@@ -17258,6 +18068,11 @@
       </c>
       <c r="T183" t="inlineStr">
         <is>
+          <t>Fortuna Sittard Stadion</t>
+        </is>
+      </c>
+      <c r="U183" t="inlineStr">
+        <is>
           <t>[['Fortuna Sittard', '3ebril33e08ddzob4bhq8awsr', 1, 10, 'Ximo Navarro'], ['Feyenoord', '20vymiy7bo8wkyxai3ew494fz', 1, 16, 'M. Wieffer'], ['Feyenoord', '20vymiy7bo8wkyxai3ew494fz', 1, 43, 'S. Giménez'], ['Fortuna Sittard', '3ebril33e08ddzob4bhq8awsr', 2, 48, 'Deroy Duarte'], ['Feyenoord', '20vymiy7bo8wkyxai3ew494fz', 2, 63, 'Igor Paixão'], ['Fortuna Sittard', '3ebril33e08ddzob4bhq8awsr', 2, 84, 'D. Siovas']]</t>
         </is>
       </c>
@@ -17352,6 +18167,11 @@
       </c>
       <c r="T184" t="inlineStr">
         <is>
+          <t>Johan Cruijff Arena</t>
+        </is>
+      </c>
+      <c r="U184" t="inlineStr">
+        <is>
           <t>[['Ajax', 'd0zdg647gvgc95xdtk1vpbkys', 2, 52, 'M. Kudus']]</t>
         </is>
       </c>
@@ -17445,6 +18265,11 @@
         </is>
       </c>
       <c r="T185" t="inlineStr">
+        <is>
+          <t>Van Donge &amp; De Roo Stadion</t>
+        </is>
+      </c>
+      <c r="U185" t="inlineStr">
         <is>
           <t>[['Excelsior', 'dqk062lu0vm8epvytbm6r4mmf', 1, 20, 'R. El Yaakoubi'], ['Excelsior', 'dqk062lu0vm8epvytbm6r4mmf', 1, 45, 'C. Driouech'], ['Sparta Rotterdam', '89w5c6pw7vn0dxypi61tt0g4k', 2, 49, 'K. Saito'], ['Sparta Rotterdam', '89w5c6pw7vn0dxypi61tt0g4k', 2, 56, 'T. Lauritsen'], ['Sparta Rotterdam', '89w5c6pw7vn0dxypi61tt0g4k', 2, 60, 'B. Vriends']]</t>
         </is>
@@ -17541,6 +18366,11 @@
         </is>
       </c>
       <c r="T186" t="inlineStr">
+        <is>
+          <t>De Grolsch Veste</t>
+        </is>
+      </c>
+      <c r="U186" t="inlineStr">
         <is>
           <t>[['Twente', '4tic29sox7m39fy1ztgv0jsiq', 1, 25, 'M. Hilgers'], ['Twente', '4tic29sox7m39fy1ztgv0jsiq', 1, 34, 'R. Pröpper'], ['Twente', '4tic29sox7m39fy1ztgv0jsiq', 2, 48, 'M. Ugalde'], ['Twente', '4tic29sox7m39fy1ztgv0jsiq', 2, 55, 'V. Černý'], ['Heerenveen', '4vd2t5schmvvufrfib7f2vjdf', 2, 59, 'M. van Ewijk'], ['Heerenveen', '4vd2t5schmvvufrfib7f2vjdf', 2, 90, 'R. Kaib']]</t>
         </is>
@@ -17639,6 +18469,11 @@
         </is>
       </c>
       <c r="T187" t="inlineStr">
+        <is>
+          <t>Stadion Galgenwaard</t>
+        </is>
+      </c>
+      <c r="U187" t="inlineStr">
         <is>
           <t>[['Utrecht', 'ccpscwdcm65czscrun048ecn5', 2, 59, 'T. Douvikas'], ['Fortuna Sittard', '3ebril33e08ddzob4bhq8awsr', 2, 68, 'K. Bistrović'], ['Fortuna Sittard', '3ebril33e08ddzob4bhq8awsr', 2, 87, 'T. Noslin']]</t>
         </is>
@@ -17740,6 +18575,11 @@
       </c>
       <c r="T188" t="inlineStr">
         <is>
+          <t>Stadion Feijenoord</t>
+        </is>
+      </c>
+      <c r="U188" t="inlineStr">
+        <is>
           <t>[['Feyenoord', '20vymiy7bo8wkyxai3ew494fz', 2, 88, 'O. Idrissi']]</t>
         </is>
       </c>
@@ -17836,6 +18676,11 @@
         </is>
       </c>
       <c r="T189" t="inlineStr">
+        <is>
+          <t>Mandemakers Stadion</t>
+        </is>
+      </c>
+      <c r="U189" t="inlineStr">
         <is>
           <t>[['PSV', '24fvcruwqrqvqa3aonf8c3zuy', 1, 35, 'J. Bakayoko']]</t>
         </is>
@@ -17935,6 +18780,11 @@
       </c>
       <c r="T190" t="inlineStr">
         <is>
+          <t>Kras Stadion</t>
+        </is>
+      </c>
+      <c r="U190" t="inlineStr">
+        <is>
           <t>[['Volendam', '6g9qrm72224jrk6tkxxxi8a9n', 2, 46, 'F. Stanković'], ['Volendam', '6g9qrm72224jrk6tkxxxi8a9n', 2, 67, 'B. Benamar'], ['Volendam', '6g9qrm72224jrk6tkxxxi8a9n', 2, 88, 'B. Ould-Chikh'], ['Volendam', '6g9qrm72224jrk6tkxxxi8a9n', 2, 92, 'D. van Mieghem']]</t>
         </is>
       </c>
@@ -18032,6 +18882,11 @@
       </c>
       <c r="T191" t="inlineStr">
         <is>
+          <t>AFAS Stadion</t>
+        </is>
+      </c>
+      <c r="U191" t="inlineStr">
+        <is>
           <t>[['AZ', '3kfktv64h7kg7zryax1wktr5r', 1, 4, 'J. Karlsson']]</t>
         </is>
       </c>
@@ -18128,6 +18983,11 @@
       </c>
       <c r="T192" t="inlineStr">
         <is>
+          <t>De Oude Meerdijk</t>
+        </is>
+      </c>
+      <c r="U192" t="inlineStr">
+        <is>
           <t>[['Emmen', '3t0vjqtxc8wpjzv82i3oi2ova', 2, 63, 'O. Romeny'], ['Emmen', '3t0vjqtxc8wpjzv82i3oi2ova', 2, 71, 'O. Romeny']]</t>
         </is>
       </c>
@@ -18222,6 +19082,11 @@
       </c>
       <c r="T193" t="inlineStr">
         <is>
+          <t>Stadion Feijenoord</t>
+        </is>
+      </c>
+      <c r="U193" t="inlineStr">
+        <is>
           <t>[['Volendam', '6g9qrm72224jrk6tkxxxi8a9n', 1, 12, 'D. van Mieghem'], ['Feyenoord', '20vymiy7bo8wkyxai3ew494fz', 2, 52, 'S. Giménez'], ['Volendam', '6g9qrm72224jrk6tkxxxi8a9n', 2, 74, 'D. Mirani']]</t>
         </is>
       </c>
@@ -18314,6 +19179,11 @@
         </is>
       </c>
       <c r="T194" t="inlineStr">
+        <is>
+          <t>Fortuna Sittard Stadion</t>
+        </is>
+      </c>
+      <c r="U194" t="inlineStr">
         <is>
           <t>[['Twente', '4tic29sox7m39fy1ztgv0jsiq', 2, 67, 'V. Černý'], ['Twente', '4tic29sox7m39fy1ztgv0jsiq', 2, 71, 'M. Ugalde'], ['Twente', '4tic29sox7m39fy1ztgv0jsiq', 2, 77, 'M. Ugalde']]</t>
         </is>
@@ -18408,6 +19278,11 @@
         </is>
       </c>
       <c r="T195" t="inlineStr">
+        <is>
+          <t>Goffertstadion</t>
+        </is>
+      </c>
+      <c r="U195" t="inlineStr">
         <is>
           <t>[['NEC', '8iawijq7s9s6d85mjz8wdslki', 1, 31, 'L. Dimata'], ['NEC', '8iawijq7s9s6d85mjz8wdslki', 2, 48, 'L. Dimata'], ['Utrecht', 'ccpscwdcm65czscrun048ecn5', 2, 63, 'B. Dost'], ['Utrecht', 'ccpscwdcm65czscrun048ecn5', 2, 67, 'O. Boussaid']]</t>
         </is>
@@ -18506,6 +19381,11 @@
       </c>
       <c r="T196" t="inlineStr">
         <is>
+          <t>Philips Stadion</t>
+        </is>
+      </c>
+      <c r="U196" t="inlineStr">
+        <is>
           <t>[['Cambuur', 'ears40cp6opsgvhsy0dgyszpd', 1, 22, 'R. Balk'], ['PSV', '24fvcruwqrqvqa3aonf8c3zuy', 1, 25, 'X. Simons'], ['PSV', '24fvcruwqrqvqa3aonf8c3zuy', 2, 54, 'P. van Aanholt'], ['PSV', '24fvcruwqrqvqa3aonf8c3zuy', 2, 56, 'A. El Ghazi'], ['PSV', '24fvcruwqrqvqa3aonf8c3zuy', 2, 61, 'I. Sangaré'], ['PSV', '24fvcruwqrqvqa3aonf8c3zuy', 2, 65, 'Fábio Silva'], ['PSV', '24fvcruwqrqvqa3aonf8c3zuy', 2, 88, 'A. El Ghazi']]</t>
         </is>
       </c>
@@ -18601,6 +19481,11 @@
         </is>
       </c>
       <c r="T197" t="inlineStr">
+        <is>
+          <t>Sparta-Stadion Het Kasteel</t>
+        </is>
+      </c>
+      <c r="U197" t="inlineStr">
         <is>
           <t>[['Vitesse', '6hsriqr3ybvyg94w2k19oal50', 1, 7, 'D. Oroz'], ['Sparta Rotterdam', '89w5c6pw7vn0dxypi61tt0g4k', 1, 11, 'A. Verschueren'], ['Sparta Rotterdam', '89w5c6pw7vn0dxypi61tt0g4k', 1, 45, 'K. Saito'], ['Sparta Rotterdam', '89w5c6pw7vn0dxypi61tt0g4k', 2, 87, 'J. Kitolano']]</t>
         </is>
@@ -18699,6 +19584,11 @@
         </is>
       </c>
       <c r="T198" t="inlineStr">
+        <is>
+          <t>Abe Lenstra Stadion</t>
+        </is>
+      </c>
+      <c r="U198" t="inlineStr">
         <is>
           <t>[['Ajax', 'd0zdg647gvgc95xdtk1vpbkys', 1, 10, 'M. Kudus'], ['Ajax', 'd0zdg647gvgc95xdtk1vpbkys', 1, 16, 'E. Álvarez'], ['Ajax', 'd0zdg647gvgc95xdtk1vpbkys', 1, 19, 'S. Bergwijn'], ['Heerenveen', '4vd2t5schmvvufrfib7f2vjdf', 1, 42, 'P. van Amersfoort'], ['Ajax', 'd0zdg647gvgc95xdtk1vpbkys', 2, 52, 'K. Taylor'], ['Heerenveen', '4vd2t5schmvvufrfib7f2vjdf', 2, 79, 'S. van Hooijdonk']]</t>
         </is>
@@ -18804,6 +19694,11 @@
       </c>
       <c r="T199" t="inlineStr">
         <is>
+          <t>Johan Cruijff Arena</t>
+        </is>
+      </c>
+      <c r="U199" t="inlineStr">
+        <is>
           <t>[['Feyenoord', '20vymiy7bo8wkyxai3ew494fz', 1, 5, 'S. Giménez'], ['Ajax', 'd0zdg647gvgc95xdtk1vpbkys', 1, 17, 'E. Álvarez'], ['Ajax', 'd0zdg647gvgc95xdtk1vpbkys', 1, 37, 'D. Tadić'], ['Feyenoord', '20vymiy7bo8wkyxai3ew494fz', 2, 52, 'S. Szymański'], ['Feyenoord', '20vymiy7bo8wkyxai3ew494fz', 2, 86, 'L. Geertruida']]</t>
         </is>
       </c>
@@ -18897,6 +19792,11 @@
         </is>
       </c>
       <c r="T200" t="inlineStr">
+        <is>
+          <t>De Oude Meerdijk</t>
+        </is>
+      </c>
+      <c r="U200" t="inlineStr">
         <is>
           <t>[['Sparta Rotterdam', '89w5c6pw7vn0dxypi61tt0g4k', 1, 44, 'K. Saito'], ['Sparta Rotterdam', '89w5c6pw7vn0dxypi61tt0g4k', 2, 89, 'V. van Crooij']]</t>
         </is>
@@ -18996,6 +19896,11 @@
       </c>
       <c r="T201" t="inlineStr">
         <is>
+          <t>Euroborg</t>
+        </is>
+      </c>
+      <c r="U201" t="inlineStr">
+        <is>
           <t>[['Heerenveen', '4vd2t5schmvvufrfib7f2vjdf', 1, 27, 'S. van Hooijdonk'], ['Heerenveen', '4vd2t5schmvvufrfib7f2vjdf', 1, 40, 'S. van Hooijdonk']]</t>
         </is>
       </c>
@@ -19089,6 +19994,11 @@
         </is>
       </c>
       <c r="T202" t="inlineStr">
+        <is>
+          <t>De Grolsch Veste</t>
+        </is>
+      </c>
+      <c r="U202" t="inlineStr">
         <is>
           <t>[['Twente', '4tic29sox7m39fy1ztgv0jsiq', 1, 8, 'M. Ugalde'], ['Twente', '4tic29sox7m39fy1ztgv0jsiq', 1, 11, 'M. Ugalde'], ['AZ', '3kfktv64h7kg7zryax1wktr5r', 2, 66, 'J. Karlsson']]</t>
         </is>
@@ -19187,6 +20097,11 @@
       </c>
       <c r="T203" t="inlineStr">
         <is>
+          <t>Stadion Galgenwaard</t>
+        </is>
+      </c>
+      <c r="U203" t="inlineStr">
+        <is>
           <t>[['Utrecht', 'ccpscwdcm65czscrun048ecn5', 1, 41, 'T. Douvikas'], ['Go Ahead Eagles', 'b79uipsy57y1jqpy07h4i5ovk', 1, 48, 'O. Edvardsen'], ['Go Ahead Eagles', 'b79uipsy57y1jqpy07h4i5ovk', 2, 94, 'W. Willumsson']]</t>
         </is>
       </c>
@@ -19282,6 +20197,11 @@
       </c>
       <c r="T204" t="inlineStr">
         <is>
+          <t>Mandemakers Stadion</t>
+        </is>
+      </c>
+      <c r="U204" t="inlineStr">
+        <is>
           <t>[['NEC', '8iawijq7s9s6d85mjz8wdslki', 1, 18, 'O. Tannane'], ['NEC', '8iawijq7s9s6d85mjz8wdslki', 1, 26, 'E. Tavşan'], ['NEC', '8iawijq7s9s6d85mjz8wdslki', 1, 31, 'O. Tannane'], ['RKC Waalwijk', 'ed5nwjz5za3oyi20nxzgqivmx', 2, 61, 'V. Anita']]</t>
         </is>
       </c>

</xml_diff>